<commit_message>
Expand rationale for politicians
branch:
</commit_message>
<xml_diff>
--- a/tests/test_resources/test_namescan/test_namescan-explained.xlsx
+++ b/tests/test_resources/test_namescan/test_namescan-explained.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>637098719012229238</t>
+          <t>4558967249527932496</t>
         </is>
       </c>
       <c r="J2" t="b">
@@ -541,7 +541,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Muhammad Ali DURGHAM: Not an Indonesian name: محمد علي, Muhammad Yousuf Ali: Deceased 1998, Muhammad Rapsel Ali: Politician for Nasdem Party, Ali Nasir Muhammad: Not an Indonesian name: علي ناصر محمد, Muhammad Yusuf Ali: Deceased 1998-12-01, Muhammad Ali Ridha: Politician for Golongan Karya Party, Muhammad Ali Malkani: Politician for Pakistan Peoples Party, Muhammad Ali DURGHAM: Not an Indonesian name: محمد علي, Mohammed Ali NASR: Not an Indonesian name: محمد علي نصر, Mohammed Ali NASR: Not an Indonesian name: محمد علي نصر, Muhammad Shujat Ali: Deceased 2007-04-01, Mohammad Ali JAFARI: Not an Indonesian name: محمد علي جعفري, Iqbal Muhammad Ali Khan: Deceased 2022-04-19, Malek ALI: Syrian conflict, Akram Muhammad AL-SALTI: Public figure: Commander-in-Chief and Chief of Staff of the Palestine Liberation Army, Muhammad AL-QATIRJI: Syrian conflict, Muhammad Alwi Dahlan: Politician, Muhammad Rudini Darwan Ali: Politician, Muhammad Unais Ali Hisyam: Politician, Habib Muhammad Ali Al'habsyi: Politician, Mohammad Ali Shah: Deceased 2013-02-04, K.H. MUH. UNAIS ALI HISYAM, M.Pd.I: Public figure: Member of Dewan Perwakilan Rakyat (National Awakening Party Faction), Muhammad Ibrahim al-Shaar: Syrian conflict, ALI KONY: Public figure: Deputy, Lord’s Resistance Army, Mohammad Ali Jinnah: Deceased 1948-09-11, Husayn Muhamad Husayn al-Juaythini: Foreigner: PALESTINIAN TERRITORY, Occupied, Mohammadian Abbas-Ali: Not an Indonesian name: Мохаммадян Аббас-Али, Ali Ahsan Mohammad Mojaheed: Deceased 2015-11-22, Mohammad Ali ZANJIREI: Public figure: Senior advisor to Head and Deputy Head of Iran's Prisons Organisation, Mohammad Ali JAFARI: Public figure: Former Commander of the IRGC. Currently head of the Hazrat Baqiatollah al-Azam Cultural and Social 
+          <t>Muhammad Ali DURGHAM: Not an Indonesian name: محمد علي, Muhammad Yousuf Ali: Deceased 1998, Muhammad Rapsel Ali: Politician, Muhammad Rapsel Ali, male, born 1971-05-06 for Nasdem Party, Ali Nasir Muhammad: Not an Indonesian name: علي ناصر محمد, Muhammad Yusuf Ali: Deceased 1998-12-01, Muhammad Ali Ridha: Politician, Muhammad Ali Ridha, male, born 1971-02-04 for Golongan Karya Party, Muhammad Ali Malkani: Politician, Muhammad Ali Malkani, male, born 1966-11-22 for Pakistan Peoples Party, Muhammad Ali DURGHAM: Not an Indonesian name: محمد علي, Mohammed Ali NASR: Not an Indonesian name: محمد علي نصر, Mohammed Ali NASR: Not an Indonesian name: محمد علي نصر, Muhammad Shujat Ali: Deceased 2007-04-01, Mohammad Ali JAFARI: Not an Indonesian name: محمد علي جعفري, Iqbal Muhammad Ali Khan: Deceased 2022-04-19, Malek ALI: Syrian conflict, Akram Muhammad AL-SALTI: Public figure: Commander-in-Chief and Chief of Staff of the Palestine Liberation Army, Muhammad AL-QATIRJI: Syrian conflict, Muhammad Alwi Dahlan: Politician, Muhammad Alwi Dahlan, male, born 1933-05-15, in Padang, Muhammad Rudini Darwan Ali: Politician, Muhammad Rudini Darwan Ali, male, born 1986-05-09, Muhammad Unais Ali Hisyam: Politician, Muhammad Unais Ali Hisyam, male, born 1973-12-14, in , Habib Muhammad Ali Al'habsyi: Politician, Habib Muhammad Ali Al'habsyi, male, born 1969-07-16, Mohammad Ali Shah: Deceased 2013-02-04, K.H. MUH. UNAIS ALI HISYAM, M.Pd.I: Public figure: Member of Dewan Perwakilan Rakyat (National Awakening Party Faction), Muhammad Ibrahim al-Shaar: Syrian conflict, ALI KONY: Public figure: Deputy, Lord’s Resistance Army, Mohammad Ali Jinnah: Deceased 1948-09-11, Husayn Muhamad Husayn al-Juaythini: Foreigner: PALESTINIAN TERRITORY, Occupied, Mohammadian Abbas-Ali: Not an Indonesian name: Мохаммадян Аббас-Али, Ali Ahsan Mohammad Mojaheed: Deceased 2015-11-22, Mohammad Ali ZANJIREI: Public figure: Senior advisor to Head and Deputy Head of Iran's Prisons Organisation, Mohammad Ali JAFARI: Public figure: Former Commander of the IRGC. Currently head of the Hazrat Baqiatollah al-Azam Cultural and Social 
 Headquarters., Mohammad Ali JAFARI: Public figure: Former Commander of the IRGC. Currently head of the Hazrat Baqiatollah al-Azam Cultural and Social 
 Headquarters.</t>
         </is>
@@ -557,11 +557,11 @@
 Justification: Secretary-general of the World Holocaust Foundation, established at the International Conference to Review the Global Vision of the Holocaust in 2006, which Ramin was responsible for organising on behalf of the Iranian Government. Main figure responsible for censorship as Vice-Minister in charge of the Press up to Dec 2013, being directly responsible for the closure of many reforming newspapers (Etemad, Etemad-e Melli, Shargh, etc), closure of the Independent Press Syndicate and the intimidation or arrest of journalists.
 Sanctions: art. 7 (Financial sanctions) and art. 11 (Prohibition to honour certain claims), annex 7, Zanjirei Mohammad-Ali: Foreign identifier: 32.
 Justification: As Senior advisor to Head, and Deputy Head of Iran's Prisons Organisation, responsible for serious human rights violations against prisoners. Administered a system in which prisoners suffered abuse, torture and inhuman/degrading treatment and were accommodated in very poor living conditions.
-Sanctions: art. 7 (Financial sanctions) and art. 11 (Prohibition to honour certain claims), annex 7, Anwar Mohammed ZBOUN: Anwar Muhammad AL-ZBOUN, Jafari Mohammad Ali: Foreign identifier: 28.
+Sanctions: art. 7 (Financial sanctions) and art. 11 (Prohibition to honour certain claims), annex 7, Anwar Mohammed ZBOUN: Anwar Muhammad AL-ZBOUN, born 1968, in , Jafari Mohammad Ali: Foreign identifier: 28.
 Justification: Former Commander of the IRGC. Currently head of the Hazrat Baqiatollah al-Azam Cultural and Social Headquarters.
 Sanctions: art. 7 (Financial sanctions), art. 10 (Travel ban) and art. 11 (Prohibition to honour certain claims), annex 6, ALI KHANAMAN MOHAMMADI: Effective Date:05/04/2016; Expiration Date:08/25/2025; Standard Order:Y; Action:FR NOTICE ADDED; FR Citation:81.F.R. 28822 5/10/2016; , Houej Mohamad Ali: Justification: Minister for Industry, Economy and Trade in Colonel Qadhafi's Government. Closely associated with the former regime of Muammar Qadhafi.
 Sanctions: article 2 paragraph 1 (Financial sanctions), annex 3 (part A: individuals, part B: entities and organizations), Houej Mohamad Ali: Justification: Minister for Industry, Economy and Trade in Colonel Qadhafi’s Government. Closely associated with the former regime of Muammar Qadhafi.
-Sanctions: art. 4 (Travel ban), annex 5, Mohamad Ali HOUEJ: Minister for Industry, Economy and Trade in Muammar Qadhafi’s Government., Amr ARMANAZI: Amr Muhammad Najib AL-ARMANAZI, Amr Najib ARMANAZI, Mohammadreza Ali AKBARI: (Linked To: QASEMI, Rostam)</t>
+Sanctions: art. 4 (Travel ban), annex 5, Mohamad Ali HOUEJ: Minister for Industry, Economy and Trade in Muammar Qadhafi’s Government., Amr ARMANAZI: Amr Muhammad Najib AL-ARMANAZI, Amr Najib ARMANAZI, born 07 Feb 1944, Mohammadreza Ali AKBARI: (Linked To: QASEMI, Rostam)</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2105438810666735548</t>
+          <t>9081041506290180432</t>
         </is>
       </c>
       <c r="J3" t="b">
@@ -607,7 +607,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Mohammad Yahiya Moalla Dr.: Not an Indonesian name: محمد يحيى معلا, Amr Armanazi: Syrian conflict, Ahmad Ballul: Not an Indonesian name: أحمد بالول, Mohammad Mufleh: Not an Indonesian name: محمد مفلح, Imad Mohammad Deeb Khamis: Not an Indonesian name: عماد محمد ديب خميس, Mohammed Bilal Brigadier General: Syrian conflict, Mohammed Ali Nasr General: Not an Indonesian name: محمد علي نصر, Mohammad Abdul-Sattar Al Sayed Dr.: Not an Indonesian name: محمد عبد الستار السيد, S. Muhammad: Politician for National Awakening Party, Muhammed Zamrini Brigadier-General: Not an Indonesian name: محمد زمريني, Muhamad: Politician, Muhammadong: Politician for Great Indonesia Movement Party, Muhammad Yousef Hasouri Brigadier General: Not an Indonesian name: محمد يوسف حاصوري, Mohamed Maaruf Brigadier General: Not an Indonesian name: محمد معروف, Mohamad Ghazi Jalali: Syrian conflict, Jihad Mohamed Sultan Brigadier General: Not an Indonesian name: جهاد محمد سلطان, Mohamed Khaddor Major General: Not an Indonesian name: محمد خضور, Muhammad Ali Durgham Major General: Not an Indonesian name: محمد علي, Mohammed Jabir: Not an Indonesian name: محمد جابر, Mohamed Heikmat Ibrahim: Not an Indonesian name: محمد حكمت إبراهيم, Mohamad Fayez Barcha: Not an Indonesian name: محمد فايز برشة, Mohamad Amer Mardini: Syrian conflict, MuhammadAriLaw: Politician</t>
+          <t>Mohammad Yahiya Moalla Dr.: Not an Indonesian name: محمد يحيى معلا, Amr Armanazi: Syrian conflict, Ahmad Ballul: Not an Indonesian name: أحمد بالول, Mohammad Mufleh: Not an Indonesian name: محمد مفلح, Imad Mohammad Deeb Khamis: Not an Indonesian name: عماد محمد ديب خميس, Mohammed Bilal Brigadier General: Syrian conflict, Mohammed Ali Nasr General: Not an Indonesian name: محمد علي نصر, Mohammad Abdul-Sattar Al Sayed Dr.: Not an Indonesian name: محمد عبد الستار السيد, S. Muhammad: Politician, S. Muhammad, male, born 1960-04-25, in Gresik for National Awakening Party, Muhammed Zamrini Brigadier-General: Not an Indonesian name: محمد زمريني, Muhamad: Politician, Muhamad, male, born 1964-04-06, Muhammadong: Politician, Muhammadong, male, born 1969-01-09 for Great Indonesia Movement Party, Muhammad Yousef Hasouri Brigadier General: Not an Indonesian name: محمد يوسف حاصوري, Mohamed Maaruf Brigadier General: Not an Indonesian name: محمد معروف, Mohamad Ghazi Jalali: Syrian conflict, Jihad Mohamed Sultan Brigadier General: Not an Indonesian name: جهاد محمد سلطان, Mohamed Khaddor Major General: Not an Indonesian name: محمد خضور, Muhammad Ali Durgham Major General: Not an Indonesian name: محمد علي, Mohammed Jabir: Not an Indonesian name: محمد جابر, Mohamed Heikmat Ibrahim: Not an Indonesian name: محمد حكمت إبراهيم, Mohamad Fayez Barcha: Not an Indonesian name: محمد فايز برشة, Mohamad Amer Mardini: Syrian conflict, MuhammadAriLaw: Politician, Muhammad Ari Pratomo, male, born 1982-06-21</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -645,7 +645,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>14038090076280157736</t>
+          <t>7394138728020829710</t>
         </is>
       </c>
       <c r="J4" t="b">
@@ -658,7 +658,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Abdul Aziz: Deceased 1990-06-05, Abdul Aziz: Politician, Abdul Aziz: Politician, Abdul Aziz: Politician for United Development Party, H. ABDUL AZIZ, S.E.: Public figure: Member of Dewan Perwakilan Rakyat (United Development Party Faction), Abdul Azis Suseno: Politician for Prosperous Justice Party, Abdul Azis Halid: Politician for Golongan Karya Party, Abdul Azis Khafia: Politician, Abdul Azis Hasan: Politician for People's Conscience Party, Sheikh Abdul Aziz: Deceased 2008-08-11, Abdul Aziz Abbasin: Not an Indonesian name: عبد العزيز عباسین, Abdul Aziz Kamis: Politician, Abdul Aziz Junejo: Politician for Pakistan Peoples Party, Abdul Aziz Mia: Politician for Bangladesh Jamaat-e-Islami, Abdul Aziz Khandaker: Deceased 1991, Abdul Aziz Angkat: Deceased 2009-02-03, Aziz Abdullaev: Not an Indonesian name: Азиз Рефатович Абдуллаев, Dawood Ibrahim Kaskar: Foreigner: India</t>
+          <t>Abdul Aziz: Deceased 1990-06-05, Abdul Aziz: Politician, Abdul Aziz, male, born 1969, Abdul Aziz: Politician, Abdul Aziz, male, born 1972-10-12, Abdul Aziz: Politician, Abdul Aziz, male, born 1970-06-04, in Jakarta for United Development Party, H. ABDUL AZIZ, S.E.: Public figure: Member of Dewan Perwakilan Rakyat (United Development Party Faction), Abdul Azis Suseno: Politician, Abdul Aziz Suseno, male, born 1965-05-10, in Blitar for Prosperous Justice Party, Abdul Azis Halid: Politician, Abdul Azis Halid, male, born 1968-11-25 for Golongan Karya Party, Abdul Azis Khafia: Politician, Abdul Azis Khafia, male, born 1975-11-23, Abdul Azis Hasan: Politician, Abdul Azis Hasan, male, born 1967-06-30, in Ujung Pandang for People's Conscience Party, Sheikh Abdul Aziz: Deceased 2008-08-11, Abdul Aziz Abbasin: Not an Indonesian name: عبد العزيز عباسین, Abdul Aziz Kamis: Politician, Abdul Aziz Kamis, male, born 1961-11-06, Abdul Aziz Junejo: Politician, Abdul Aziz Junejo, male, born 1961-12-07 for Pakistan Peoples Party, Abdul Aziz Mia: Politician, Abdul Aziz Mia, male, born 1955 for Bangladesh Jamaat-e-Islami, Abdul Aziz Khandaker: Deceased 1991, Abdul Aziz Angkat: Deceased 2009-02-03, Aziz Abdullaev: Not an Indonesian name: Азиз Рефатович Абдуллаев, Dawood Ibrahim Kaskar: Foreigner: India</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -705,7 +705,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>15310107934662735601</t>
+          <t>13477009712307192955</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -718,12 +718,12 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Subhi Ahmad Al Abdallah: Not an Indonesian name: صبحي أحمد العبدالله, Khalaf Souleymane Abdallah: Syrian conflict, Abdillah: Politician, Abdillah: Politician, ABDALLAH: Syrian conflict, Abdullah Berri: Not an Indonesian name: عبدالله بري, Abdullah Khaleel Hussein: Not an Indonesian name: عبدالله خليل حسين, Ali Abdullah Ayyub: Not an Indonesian name: علي عبدالله أيوب, MUSA HILAL ABDALLA ALNSIEM: Foreigner: Sudan, Edward Ğabdullacanof: Not an Indonesian name: Edvard Yunusovič, AL-ABDALLAH: Syrian conflict, Suhail Al-Abdullah Brigadier General: Not an Indonesian name: سهيل العبدالله</t>
+          <t>Subhi Ahmad Al Abdallah: Not an Indonesian name: صبحي أحمد العبدالله, Khalaf Souleymane Abdallah: Syrian conflict, Abdillah: Politician, Abdillah, male, born 1955-05-19, in Medan, Abdillah: Politician, Abdillah, male, born 1965-05-26, ABDALLAH: Syrian conflict, Abdullah Berri: Not an Indonesian name: عبدالله بري, Abdullah Khaleel Hussein: Not an Indonesian name: عبدالله خليل حسين, Ali Abdullah Ayyub: Not an Indonesian name: علي عبدالله أيوب, MUSA HILAL ABDALLA ALNSIEM: Foreigner: Sudan, Edward Ğabdullacanof: Not an Indonesian name: Edvard Yunusovič, AL-ABDALLAH: Syrian conflict, Suhail Al-Abdullah Brigadier General: Not an Indonesian name: سهيل العبدالله</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Abdulla: Sheikh Tameem, Pak Ud: Date of designation referred to in Article 7d(2)(i): 16.5.2005., Aris Sumarsono: Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 7 Jun. 2018. Review pursuant to Security Council resolution 2368 (2017) was concluded on 15 November 2021., ABDUL: (UK Sanctions List Ref):AQD0344. (UN Ref):QDi.187. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 7 Jun. 2018. Review pursuant to Security Council resolution 2368 (2017) was concluded on 15 November 2021. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals
+          <t>Abdulla: Sheikh Tameem, born 2000-11-11, in , Pak Ud: Date of designation referred to in Article 7d(2)(i): 16.5.2005., Aris Sumarsono: Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 7 Jun. 2018. Review pursuant to Security Council resolution 2368 (2017) was concluded on 15 November 2021., ABDUL: (UK Sanctions List Ref):AQD0344. (UN Ref):QDi.187. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 7 Jun. 2018. Review pursuant to Security Council resolution 2368 (2017) was concluded on 15 November 2021. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals
 Listed On: 18/05/2005;
 Date Designated: 16/05/2005;, Pak Ud: Date of designation referred to in Article 7d(2)(i): 16.5.2005., FAKER BEN ABDELAZZIZ BOUSSORA: Eyes: dark;
 Hair: black;
@@ -771,7 +771,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>11294957231092013345</t>
+          <t>17777211603270557273</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -784,17 +784,17 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Abu Bakar: Deceased 2019-07-13, Abu Bakar Abdi: Politician, Wan Abubakar: Politician for National Mandate Party, Tagore Abubakar: Politician for Indonesian Democratic Party – Struggle, Abu Bakar Jamalia: Politician, Wan Abu Bakar: Politician for National Mandate Party, Abu Bakar Sidik: Politician, Aboe Bakar Al-Habsyi: Politician for Prosperous Justice Party, Mohammed, Shariff Omar: Foreigner: TANZANIA, UNITED REPUBLIC OF, Abu Bakr Baira: Not an Indonesian name: أبو بكر مصطفى بعيرة</t>
+          <t>Abu Bakar: Deceased 2019-07-13, Abu Bakar Abdi: Politician, Abu Bakar Abdi, male, born 1965-05-05, Wan Abubakar: Politician, Wan Abu Bakar, male, born 1950-08-09, in Selat Panjang for National Mandate Party, Tagore Abubakar: Politician, Tagore Abu Bakar, male, born 1954-04-20, in Takengon for Indonesian Democratic Party – Struggle, Abu Bakar Jamalia: Politician, Abu Bakar Jamalia, male, born 1953-07-21, Wan Abu Bakar: Politician, Wan Abu Bakar, male, born 1950-08-09 for National Mandate Party, Abu Bakar Sidik: Politician, Abu Bakar Sidik, male, born 1962-05-25, Aboe Bakar Al-Habsyi: Politician, Aboe Bakar, Habib Aboe Bakar Alhabsyi, male, born 1964-10-15, in Jakarta for Prosperous Justice Party, Mohammed, Shariff Omar: Foreigner: TANZANIA, UNITED REPUBLIC OF, Abu Bakr Baira: Not an Indonesian name: أبو بكر مصطفى بعيرة</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Abu Bakar Ba'asyir: Foreign identifier: QI.B.217.06.
+          <t xml:space="preserve">Abu Bakar Ba'asyir: Foreign identifier: QI.B.217.06.
 Sanctions: article 3 paragraphs 1 and 2 (Financial sanctions) and articles 4 and 4a (Travel ban)
 Other information: Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 Jan 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 Nov 2020. INTERPOL-UN Security Council Special Notice web link available.
-Good quality a.k.a a) Abu Bakar Baasyir, born on 17 Aug 1938 in Jombang, East Java, Indonesia; b) Abu Bakar Bashir born on 17 Aug 1938 in Jombang, East Java, Indonesia, Abu Bakar Ba'asyir: Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020., ABU BAKAR BA'ASYIR: Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals, Abu Bakar Bashir: Abdus Somad, Abu Bakar Baasyir, Abu Bakar Ba’asyir, Abdus Samad, Abu Bakar BAASYIR: (UK Sanctions List Ref):AQD0114. (UN Ref):QDi.217. Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/notice/search/un/1428633
+Good quality a.k.a a) Abu Bakar Baasyir, born on 17 Aug 1938 in Jombang, East Java, Indonesia; b) Abu Bakar Bashir born on 17 Aug 1938 in Jombang, East Java, Indonesia, Abu Bakar Ba'asyir: Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020., ABU BAKAR BA'ASYIR: Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals, Abu Bakar Bashir: Abdus Somad, Abu Bakar Baasyir, Abu Bakar Ba’asyir, Abdus Samad, born 1938-08-17, in , Abu Bakar BAASYIR: (UK Sanctions List Ref):AQD0114. (UN Ref):QDi.217. Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/notice/search/un/1428633
 Listed On: 26/04/2006;
-Date Designated: 21/04/2006;, Abu Bakar Bashir: Abdus Somad, Abu Bakar Baasyir, Abu Bakar Ba’asyir, Abdus Samad</t>
+Date Designated: 21/04/2006;, Abu Bakar Bashir: Abdus Somad, Abu Bakar Baasyir, Abu Bakar Ba’asyir, Abdus Samad, male, born 1938-08-17, in </t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>10843769054497992370</t>
+          <t>9345809663888044064</t>
         </is>
       </c>
       <c r="J7" t="b">
@@ -840,7 +840,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Mohammad Yahiya Moalla Dr.: Not an Indonesian name: محمد يحيى معلا, Imad Mohammad Deeb Khamis: Not an Indonesian name: عماد محمد ديب خميس, Mohammad Mufleh: Not an Indonesian name: محمد مفلح, Mohammed Bilal Brigadier General: Syrian conflict, Mohammad Abdul-Sattar Al Sayed Dr.: Not an Indonesian name: محمد عبد الستار السيد, Ahmad Ballul: Not an Indonesian name: أحمد بالول, Amr Armanazi: Syrian conflict, Mohammed Ali Nasr General: Not an Indonesian name: محمد علي نصر, S. Muhammad: Politician for National Awakening Party, Muhammed Zamrini Brigadier-General: Not an Indonesian name: محمد زمريني, Muhamad: Politician, Muhammadong: Politician for Great Indonesia Movement Party</t>
+          <t>Mohammad Yahiya Moalla Dr.: Not an Indonesian name: محمد يحيى معلا, Imad Mohammad Deeb Khamis: Not an Indonesian name: عماد محمد ديب خميس, Mohammad Mufleh: Not an Indonesian name: محمد مفلح, Mohammed Bilal Brigadier General: Syrian conflict, Mohammad Abdul-Sattar Al Sayed Dr.: Not an Indonesian name: محمد عبد الستار السيد, Ahmad Ballul: Not an Indonesian name: أحمد بالول, Amr Armanazi: Syrian conflict, Mohammed Ali Nasr General: Not an Indonesian name: محمد علي نصر, S. Muhammad: Politician, S. Muhammad, male, born 1960-04-25, in Gresik for National Awakening Party, Muhammed Zamrini Brigadier-General: Not an Indonesian name: محمد زمريني, Muhamad: Politician, Muhamad, male, born 1964-04-06, Muhammadong: Politician, Muhammadong, male, born 1969-01-09 for Great Indonesia Movement Party</t>
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>15201168718847166076</t>
+          <t>16787390437967957881</t>
         </is>
       </c>
       <c r="J8" t="b">
@@ -887,12 +887,12 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Ali Abdullah Ayyub: Not an Indonesian name: علي عبدالله أيوب, Abdullah Khaleel Hussein: Not an Indonesian name: عبدالله خليل حسين, Abdullah Berri: Not an Indonesian name: عبدالله بري, MUSA HILAL ABDALLA ALNSIEM: Foreigner: Sudan, ABDALLAH: Syrian conflict, Abdillah: Politician, Abdillah: Politician, Subhi Ahmad Al Abdallah: Not an Indonesian name: صبحي أحمد العبدالله, Suhail Al-Abdullah Brigadier General: Not an Indonesian name: سهيل العبدالله, Khalaf Souleymane Abdallah: Syrian conflict, AL-ABDALLAH: Syrian conflict</t>
+          <t>Ali Abdullah Ayyub: Not an Indonesian name: علي عبدالله أيوب, Abdullah Khaleel Hussein: Not an Indonesian name: عبدالله خليل حسين, Abdullah Berri: Not an Indonesian name: عبدالله بري, MUSA HILAL ABDALLA ALNSIEM: Foreigner: Sudan, ABDALLAH: Syrian conflict, Abdillah: Politician, Abdillah, male, born 1965-05-26, Abdillah: Politician, Abdillah, male, born 1955-05-19, in Medan, Subhi Ahmad Al Abdallah: Not an Indonesian name: صبحي أحمد العبدالله, Suhail Al-Abdullah Brigadier General: Not an Indonesian name: سهيل العبدالله, Khalaf Souleymane Abdallah: Syrian conflict, AL-ABDALLAH: Syrian conflict</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Abdulla: Sheikh Tameem</t>
+          <t xml:space="preserve">Abdulla: Sheikh Tameem, born 2000-11-11, in </t>
         </is>
       </c>
     </row>
@@ -925,7 +925,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>11400088041439037532</t>
+          <t>2993838869014342318</t>
         </is>
       </c>
       <c r="J9" t="b">
@@ -938,7 +938,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Suhayl Hassan: Syrian conflict, Malik Hasan: Not an Indonesian name: مالك حسن, Hossein Taeb: Not an Indonesian name: حسين طائب, Hasani: Deceased 2018-02-17, M. M. Hassan: Politician for Indian National Congress, Bassam Al Hassan: Not an Indonesian name: بسام الحسن, Ibrahim Al-Hassan Major General: Not an Indonesian name: إبراهيم الحسن, AL-HASAN: Syrian conflict, Jamil Hassan: Not an Indonesian name: جميل حسن, Nabil Al-Hasan: Not an Indonesian name: نبيل الحسن, Nabil AL-HASAN: Not an Indonesian name: حسن نبيل, Ahmed Mahmoud Hassan: Not an Indonesian name: šejk Hassan, Hassan Khan: Politician for Jammu &amp; Kashmir National Conference</t>
+          <t>Suhayl Hassan: Syrian conflict, Malik Hasan: Not an Indonesian name: مالك حسن, Hossein Taeb: Not an Indonesian name: حسين طائب, Hasani: Deceased 2018-02-17, M. M. Hassan: Politician, Malik Mohammed Hassan, male, born 1947-05-14, in Thiruvananthapuram for Indian National Congress, Bassam Al Hassan: Not an Indonesian name: بسام الحسن, Ibrahim Al-Hassan Major General: Not an Indonesian name: إبراهيم الحسن, AL-HASAN: Syrian conflict, Jamil Hassan: Not an Indonesian name: جميل حسن, Nabil Al-Hasan: Not an Indonesian name: نبيل الحسن, Nabil AL-HASAN: Not an Indonesian name: حسن نبيل, Ahmed Mahmoud Hassan: Not an Indonesian name: šejk Hassan, Hassan Khan: Politician, Haji Ghulam Hassan Khan, male, born 1936-12-11 for Jammu &amp; Kashmir National Conference</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>6663502817338257970</t>
+          <t>6576989606114601390</t>
         </is>
       </c>
       <c r="J10" t="b">
@@ -985,12 +985,12 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Ahmed al-Jarroucheh Major General: Not an Indonesian name: أحمد الجاروشة, Ahmed Khalil Khalil: Not an Indonesian name: احمد خليل خليل, Ghassan Ahmed Ghannam: Syrian conflict, Ahmed Dibe: Not an Indonesian name: أحمد ديب, Ahmad: Politician, Ahmad Tohari: Politician, Ahmad Sayyed: Not an Indonesian name: أحمد السيد, Riad al-Ahmed Major General: Not an Indonesian name: رياض الأحمد, Jawdat al-Ahmed Brigadier General: Not an Indonesian name: جودت الأحمد, Mohammed al-Ahmed: Not an Indonesian name: محمد الأحمد, Ahmad AL-SAYED: Syrian conflict</t>
+          <t>Ahmed al-Jarroucheh Major General: Not an Indonesian name: أحمد الجاروشة, Ahmed Khalil Khalil: Not an Indonesian name: احمد خليل خليل, Ghassan Ahmed Ghannam: Syrian conflict, Ahmed Dibe: Not an Indonesian name: أحمد ديب, Ahmad: Politician, Ahmad, male, born 1966-11-27, Ahmad Tohari: Politician, Ahmad, male, born 1948-06-13, in , Ahmad Sayyed: Not an Indonesian name: أحمد السيد, Riad al-Ahmed Major General: Not an Indonesian name: رياض الأحمد, Jawdat al-Ahmed Brigadier General: Not an Indonesian name: جودت الأحمد, Mohammed al-Ahmed: Not an Indonesian name: محمد الأحمد, Ahmad AL-SAYED: Syrian conflict</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Khalil Yusif HARB: Sayyid AHMAD, Abu MUSTAFA, Mustafa Khalil HARB, Khalil Yusuf HARB, Hajj Ya'taqad Khalil HARB</t>
+          <t>Khalil Yusif HARB: Sayyid AHMAD, Abu MUSTAFA, Mustafa Khalil HARB, Khalil Yusuf HARB, Hajj Ya'taqad Khalil HARB, born 09 Oct 1958</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>12989259646850832884</t>
+          <t>4836203185392951978</t>
         </is>
       </c>
       <c r="J11" t="b">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>14521655500561362125</t>
+          <t>8761211111575463348</t>
         </is>
       </c>
       <c r="J12" t="b">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Mubarok: Yassin Syawal, Salim Yasin, Yasin Mahmud Mochtar, Abdul Hadi Yasin, Muhamad Mubarok, Muhammad Syawal, Yassin Sywal, Abu Seta, Mahmud, Abu Muamar, Yassin SYAWAL: Associated With: Al Qaeda;
+          <t>Mubarok: Yassin Syawal, Salim Yasin, Yasin Mahmud Mochtar, Abdul Hadi Yasin, Muhamad Mubarok, Muhammad Syawal, Yassin Sywal, Abu Seta, Mahmud, Abu Muamar, born 1962-09-03, in , Yassin SYAWAL: Associated With: Al Qaeda;
 NZ Designation Date: 1/21/2004;
 Entry Date2: 25/06/2004
 Amended 12/12/2014 SCA/2/14 (25)
@@ -1105,7 +1105,7 @@
 Other2: At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 Feb. 2019.v Review pursuant to Security Council 
 resolution 2610 (2021) was concluded on 8 November 2022. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/notice/search/un/1424789, Yassin Syawal: At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 Feb. 2019. Review pursuant to Security Council resolution 2610 (2021) was concluded on 8 November 2022., MAHMUD: (UK Sanctions List Ref):AQD0335. (UN Ref):QDi.123. At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 Feb. 2019. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/notice/search/un/1424789
 Listed On: 05/09/2003;
-Date Designated: 09/09/2003;, Mubarok: Yassin Syawal, Salim Yasin, Yasin Mahmud Mochtar, Abdul Hadi Yasin, Muhamad Mubarok, Muhammad Syawal, Yassin Sywal, Abu Seta, Mahmud, Abu Muamar, Yassin SYAWAL: ABU MUAMAR, Yasin Mahmud MOCHTAR, Muhamad MUBAROK, Muhammad SYAWAL, Abdul Hadi YASIN, Salim YASIN, ABU SETA, MAHMUD, Syawal YASIN, Laode Agussalim MUBARAK, Ustad Haji Laudi Agus Salim MUHAMMAD, Mohd Shahwal KHAN, Laode IDA, AGUS SALIM, YASSIN SYAWAL: At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 February 2019. Review pursuant to Security Council resolution 2610 (2021) was concluded on 8 November 2022. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals</t>
+Date Designated: 09/09/2003;, Mubarok: Yassin Syawal, Salim Yasin, Yasin Mahmud Mochtar, Abdul Hadi Yasin, Muhamad Mubarok, Muhammad Syawal, Yassin Sywal, Abu Seta, Mahmud, Abu Muamar, male, born 1962-09-03, in , Yassin SYAWAL: ABU MUAMAR, Yasin Mahmud MOCHTAR, Muhamad MUBAROK, Muhammad SYAWAL, Abdul Hadi YASIN, Salim YASIN, ABU SETA, MAHMUD, Syawal YASIN, Laode Agussalim MUBARAK, Ustad Haji Laudi Agus Salim MUHAMMAD, Mohd Shahwal KHAN, Laode IDA, AGUS SALIM, born 03 Sep 1962, in , YASSIN SYAWAL: At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 February 2019. Review pursuant to Security Council resolution 2610 (2021) was concluded on 8 November 2022. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>16176448678766397352</t>
+          <t>6813420260146292579</t>
         </is>
       </c>
       <c r="J13" t="b">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Ahmad Farhan Hamid: Politician for National Mandate Party, Hamid Reza EMADI: Public figure: Former Press TV Newsroom Director. Former Press TV Senior Producer., Fathi Ahmad Hammad: Politician, Najm Hamad AL AHMAD: Not an Indonesian name: نجم حمد الأحمد, Najm Hamad Al Ahmad: Syrian conflict, Najm Hamad Al Ahmad: Not an Indonesian name: نجم حمد الأحمد, Najm Hamad AL AHMAD: Not an Indonesian name: نجم حمد الأحمد</t>
+          <t>Ahmad Farhan Hamid: Politician, Ahmad Farhan Hamid, male, born 1953-01-21 for National Mandate Party, Hamid Reza EMADI: Public figure: Former Press TV Newsroom Director. Former Press TV Senior Producer., Fathi Ahmad Hammad: Politician, Fathi Ahmad Hammad, male, born 1961, Najm Hamad AL AHMAD: Not an Indonesian name: نجم حمد الأحمد, Najm Hamad Al Ahmad: Syrian conflict, Najm Hamad Al Ahmad: Not an Indonesian name: نجم حمد الأحمد, Najm Hamad AL AHMAD: Not an Indonesian name: نجم حمد الأحمد</t>
         </is>
       </c>
       <c r="M13" t="inlineStr"/>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1587103771365630393</t>
+          <t>6488034680104985054</t>
         </is>
       </c>
       <c r="J14" t="b">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Abdurrahman B.T.M: Politician, Abdurachman: Politician for Perindo Party</t>
+          <t>Abdurrahman B.T.M: Politician, Abdurrahman B.T.M, male, born 1962-06-19, Abdurachman: Politician, Abdurachman, male, born 1954-02-05 for Perindo Party</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>10154554551034933157</t>
+          <t>7761883952758496458</t>
         </is>
       </c>
       <c r="J15" t="b">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Mohammad Hatta: Deceased 1980-03-14, Muhammad Hatta: Politician, MOHAMMAD HATTA: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction), Hatta Rajasa: Politician for National Mandate Party, Mohammad Hatta: Politician for National Mandate Party, Rana Muhammad Hayat: Politician for Pakistan Muslim League (N), Muhammad Hadi Nasrallah: Deceased 1997, Mian Muhammad Akhtar Hayat: Politician for Pakistan Tehreek-e-Insaf</t>
+          <t>Mohammad Hatta: Deceased 1980-03-14, Muhammad Hatta: Politician, Muhammad Hatta, male, born 1973-08-17, in Surakarta, MOHAMMAD HATTA: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction), Hatta Rajasa: Politician, Ir. M. Hatta Rajasa, Muhammad Hatta Rajasa, male, born 1953-09-18, in Palembang for National Mandate Party, Mohammad Hatta: Politician, Mohammad Hatta, male, born 1973-08-17, in Surabaya for National Mandate Party, Rana Muhammad Hayat: Politician, Rana Muhammad Hayat Khan, male, born 1955-12-24 for Pakistan Muslim League (N), Muhammad Hadi Nasrallah: Deceased 1997, Mian Muhammad Akhtar Hayat: Politician, Mian Muhammad Akhtar Hayat, male, born 1950 for Pakistan Tehreek-e-Insaf</t>
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>15242276612243551718</t>
+          <t>8365530065398086069</t>
         </is>
       </c>
       <c r="J16" t="b">
@@ -1310,7 +1310,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Rusmin Abdul Gani: Politician, Abdul Ghani Lone: Deceased 2002-05-21, Ruslan Abdul Gani: Politician for People's Conscience Party, Emad Abdul-Ghani Sabouni: Not an Indonesian name: عماد عبدالغني صابوني, Abdul Ganie Mohamed: Politician, Abdul Ghani Baradar: Politician for Taliban, Abdul Ghani Kasuba: Politician for Prosperous Justice Party</t>
+          <t>Rusmin Abdul Gani: Politician, Rusmin Abdul Gani, male, born 1980-12-08, Abdul Ghani Lone: Deceased 2002-05-21, Ruslan Abdul Gani: Politician, Ruslan Abdul Gani, male, born 1958-12-09 for People's Conscience Party, Emad Abdul-Ghani Sabouni: Not an Indonesian name: عماد عبدالغني صابوني, Abdul Ganie Mohamed: Politician, Abdul Ganie Mohamed, male, born 1937-11-04, Abdul Ghani Baradar: Politician, Baradar, Mullah Abdul Ghani Baradar, male, born 1968-09-29, in Weetmak for Taliban, Abdul Ghani Kasuba: Politician, Abdul Ghani Kasuba, male, born 1951-12-21, in Bacan islands for Prosperous Justice Party</t>
         </is>
       </c>
       <c r="M16" t="inlineStr"/>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>3865387664075495442</t>
+          <t>208773953576434720</t>
         </is>
       </c>
       <c r="J17" t="b">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>9835759401772581940</t>
+          <t>14958980638395977557</t>
         </is>
       </c>
       <c r="J18" t="b">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>15011203119919843485</t>
+          <t>10592543599469362806</t>
         </is>
       </c>
       <c r="J19" t="b">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Mulyadi: Politician for Great Indonesia Movement Party, Mulyadi: Politician, Mulyadi: Politician for Democratic Party, Mulyadi: Politician for United Development Party, Ir. H. MULYADI: Public figure: Member of Dewan Perwakilan Rakyat (Democrat Party Faction), Muliadi: Politician</t>
+          <t>Mulyadi: Politician, Mulyadi, male, born 1970-11-02, in Bogor for Great Indonesia Movement Party, Mulyadi: Politician, Mulyadi, male, born 1970-03-01, Mulyadi: Politician, Mulyadi, male, born 1963-02-13, in Bukittinggi for Democratic Party, Mulyadi: Politician, Mulyadi, male, born 1967-05-14, in Jakarta for United Development Party, Ir. H. MULYADI: Public figure: Member of Dewan Perwakilan Rakyat (Democrat Party Faction), Muliadi: Politician, Muliadi, male, born 1970-07-07</t>
         </is>
       </c>
       <c r="M19" t="inlineStr"/>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>10273533500285644611</t>
+          <t>5443673151062899518</t>
         </is>
       </c>
       <c r="J20" t="b">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Amar Ismael: Not an Indonesian name: عمار إسماعيل, Ismael Ismael: Syrian conflict, Ezzedine Ismael: Not an Indonesian name: عزالدين إسماعيل, M. M. Ismail: Deceased 2005-01-17, Ismail: Politician</t>
+          <t>Amar Ismael: Not an Indonesian name: عمار إسماعيل, Ismael Ismael: Syrian conflict, Ezzedine Ismael: Not an Indonesian name: عزالدين إسماعيل, M. M. Ismail: Deceased 2005-01-17, Ismail: Politician, Ismail, male, born 1957-05-19</t>
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>8232724777345846402</t>
+          <t>14630247723957871873</t>
         </is>
       </c>
       <c r="J21" t="b">
@@ -1553,12 +1553,12 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Ali Barakat: Not an Indonesian name: علي بركات, Ali: Politician, Nasser Al-Ali Brigadier General: Not an Indonesian name: ناصر العلي, Aous "Ali" Aslan Major General: Not an Indonesian name: أوس "</t>
+          <t>Ali Barakat: Not an Indonesian name: علي بركات, Ali: Politician, Ali, male, born 1950-09-01, Nasser Al-Ali Brigadier General: Not an Indonesian name: ناصر العلي, Aous "Ali" Aslan Major General: Not an Indonesian name: أوس "</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Ahmad Al Ghazali: Al, Ahmad Al Ghazali Köhler, Al Ghazali</t>
+          <t>Ahmad Al Ghazali: Al, Ahmad Al Ghazali Köhler, Al Ghazali, male, born 1997-09-01, in Jakarta</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2665620287857550971</t>
+          <t>6618276129218788492</t>
         </is>
       </c>
       <c r="J22" t="b">
@@ -1604,12 +1604,12 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Ali Barakat: Not an Indonesian name: علي بركات, Ali: Politician, Nasser Al-Ali Brigadier General: Not an Indonesian name: ناصر العلي, Aous "Ali" Aslan Major General: Not an Indonesian name: أوس "</t>
+          <t>Ali Barakat: Not an Indonesian name: علي بركات, Ali: Politician, Ali, male, born 1950-09-01, Nasser Al-Ali Brigadier General: Not an Indonesian name: ناصر العلي, Aous "Ali" Aslan Major General: Not an Indonesian name: أوس "</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Ahmad Al Ghazali: Al, Ahmad Al Ghazali Köhler, Al Ghazali</t>
+          <t>Ahmad Al Ghazali: Al, Ahmad Al Ghazali Köhler, Al Ghazali, male, born 1997-09-01, in Jakarta</t>
         </is>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>5036954033414705670</t>
+          <t>14266958555859629077</t>
         </is>
       </c>
       <c r="J23" t="b">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Nasrullah: Politician for National Mandate Party, Mat Solar: Politician for United Development Party, Nasrul: Politician, Nasrullo Sayidov: Politician</t>
+          <t>Nasrullah: Politician, Nasrullah, male, born 1968-11-18, in Pekalongan for National Mandate Party, Mat Solar: Politician, Nasrullah, male, born 1962-12-04, in Jakarta for United Development Party, Nasrul: Politician, Nasrul, male, born 1967-05-14, Nasrullo Sayidov: Politician, Nasrullo Sayyid), male, born 1958-02-20</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>9462659872976603430</t>
+          <t>12972531040749141575</t>
         </is>
       </c>
       <c r="J24" t="b">
@@ -1715,7 +1715,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Rahman: Politician for United Development Party, A. Rahman: Politician for United Development Party, K. Rahman Khan: Politician for Indian National Congress, B. Raman: Deceased 2013-06-16</t>
+          <t>Rahman: Politician, Rahman, male, born 1962-01-30, in Bandung for United Development Party, A. Rahman: Politician, A. Rahman, male, born 1959-02-17 for United Development Party, K. Rahman Khan: Politician, K. Rahman Khan, male, born 1939-04-05, in Mandya for Indian National Congress, B. Raman: Deceased 2013-06-16</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -1756,7 +1756,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>9090190138349623020</t>
+          <t>11869132067293909402</t>
         </is>
       </c>
       <c r="J25" t="b">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>M.K. Anwar: Deceased 2017-10-24, Anwar: Politician, Anwar: Politician</t>
+          <t>M.K. Anwar: Deceased 2017-10-24, Anwar: Politician, Anwar, male, born 1965-08-05, Anwar: Politician, Anwar, male, born 1963-08-06</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>8631612707956702791</t>
+          <t>7066761180596573176</t>
         </is>
       </c>
       <c r="J26" t="b">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Amer al-Achi Major General: Not an Indonesian name: عامر العشي, Mahmoud Ibraheem Sa’iid Dr.: Not an Indonesian name: محمود ابراهيم سعيد, B. Ibrahim: Politician, Mohammed Ibrahim: Politician</t>
+          <t>Amer al-Achi Major General: Not an Indonesian name: عامر العشي, Mahmoud Ibraheem Sa’iid Dr.: Not an Indonesian name: محمود ابراهيم سعيد, B. Ibrahim: Politician, B. Ibrahim, male, born 1946-01-02, Mohammed Ibrahim: Politician, Moh.Ibrahim, male, born 1936</t>
         </is>
       </c>
       <c r="M26" t="inlineStr"/>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>9643103747421532263</t>
+          <t>11690031790147095061</t>
         </is>
       </c>
       <c r="J27" t="b">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Samsudin S.: Politician, Samsudin: Politician, Syamsudin: Politician, Syamsuddin Hb.: Politician for Nasdem Party</t>
+          <t>Samsudin S.: Politician, Samsudin S., male, born 1982-02-12, Samsudin: Politician, Samsudin, male, born 1962-12-01, Syamsudin: Politician, Syamsudin, male, born 1954-02-07, Syamsuddin Hb.: Politician, Syamsuddin Hb., male, born 1974-07-07 for Nasdem Party</t>
         </is>
       </c>
       <c r="M27" t="inlineStr"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>12044495675206993930</t>
+          <t>12182520774192383997</t>
         </is>
       </c>
       <c r="J28" t="b">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>R. Sudirman: Politician for Nasdem Party, Sudirman: Politician, Sudirman: Politician, Sudarmanto: Politician for Great Indonesia Movement Party</t>
+          <t>R. Sudirman: Politician, R. Sudirman, male, born 1957-12-30, in Maros for Nasdem Party, Sudirman: Politician, Sudirman, male, born 1974-11-10, Sudirman: Politician, Sudirman, male, born 1979-10-28, Sudarmanto: Politician, Sudarmanto, male, born 1957-05-15 for Great Indonesia Movement Party</t>
         </is>
       </c>
       <c r="M28" t="inlineStr"/>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>3821227053820620693</t>
+          <t>6552148137850177530</t>
         </is>
       </c>
       <c r="J29" t="b">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Sukiman: Politician, Sukiman: Politician, Sukiman: Politician for National Mandate Party, H. SUKIMAN, S. Pd., M.M.: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction)</t>
+          <t>Sukiman: Politician, Sukiman, male, born 1953-08-10, Sukiman: Politician, Sukiman, male, born 1953-08-10, in Madiun, Sukiman: Politician, Sukiman, male, born 1968-07-15, in Nanga Pak for National Mandate Party, H. SUKIMAN, S. Pd., M.M.: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction)</t>
         </is>
       </c>
       <c r="M29" t="inlineStr"/>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>6482097363916607899</t>
+          <t>17672577618118732994</t>
         </is>
       </c>
       <c r="J30" t="b">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Syamsudin: Politician, Syamsuddin Hb.: Politician for Nasdem Party, Samsudin S.: Politician, Samsudin: Politician</t>
+          <t>Syamsudin: Politician, Syamsudin, male, born 1954-02-07, Syamsuddin Hb.: Politician, Syamsuddin Hb., male, born 1974-07-07 for Nasdem Party, Samsudin S.: Politician, Samsudin S., male, born 1982-02-12, Samsudin: Politician, Samsudin, male, born 1962-12-01</t>
         </is>
       </c>
       <c r="M30" t="inlineStr"/>
@@ -2048,7 +2048,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>10959069045536230623</t>
+          <t>13934406406176155609</t>
         </is>
       </c>
       <c r="J31" t="b">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Abdul Haris: Politician, Abdul Haris: Politician, Abdul Haris Makkie: Politician</t>
+          <t>Abdul Haris: Politician, Abdul Haris, male, born 1968-05-03, Abdul Haris: Politician, Abdul Haris, male, born 1956-07-11, Abdul Haris Makkie: Politician, Abdul Haris Makkie, male, born 1962-05-10</t>
         </is>
       </c>
       <c r="M31" t="inlineStr"/>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>3789493295220278084</t>
+          <t>8830964935097315160</t>
         </is>
       </c>
       <c r="J32" t="b">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dewi Sukarno: Naoko Nemoto, Ratna Sari Dewi Sukarno, Kartika Sari Dewi Soekarno: </t>
+          <t>Dewi Sukarno: Naoko Nemoto, Ratna Sari Dewi Sukarno, female, born 1940-02-06, in Tokyo, Kartika Sari Dewi Soekarno: Kartika Sari Dewi Soekarno, female, born 1967-03-11, in Tokyo</t>
         </is>
       </c>
     </row>
@@ -2154,7 +2154,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>7965914032411116607</t>
+          <t>6546123067562796969</t>
         </is>
       </c>
       <c r="J33" t="b">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Firmandez: Politician for Golongan Karya Party, H. FIRMANDEZ: Public figure: Member of Dewan Perwakilan Rakyat (Golkar Party Faction), Firmansyah: Politician</t>
+          <t>Firmandez: Politician, Firmandez, male, born 1960-10-21, in Banda Aceh for Golongan Karya Party, H. FIRMANDEZ: Public figure: Member of Dewan Perwakilan Rakyat (Golkar Party Faction), Firmansyah: Politician, Firmansyah, male, born 1966-03-11</t>
         </is>
       </c>
       <c r="M33" t="inlineStr"/>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>11378140825670653740</t>
+          <t>811237689581992791</t>
         </is>
       </c>
       <c r="J34" t="b">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Haerudin: Politician for Crescent Star Party, HAERUDIN, S.Ag, MH: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction), Hairudin: Politician for Great Indonesia Movement Party</t>
+          <t>Haerudin: Politician, Haerudin, male, born 1974-05-28, in Garut for Crescent Star Party, HAERUDIN, S.Ag, MH: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction), Hairudin: Politician, Hairudin, male, born 1967-10-07 for Great Indonesia Movement Party</t>
         </is>
       </c>
       <c r="M34" t="inlineStr"/>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>5654746315049222703</t>
+          <t>16141970136513248035</t>
         </is>
       </c>
       <c r="J35" t="b">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Imran: Deceased 2020-03-28, Amran: Politician for National Mandate Party, AMRAN, S.E.: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction)</t>
+          <t>Imran: Deceased 2020-03-28, Amran: Politician, Amran, male, born 1968-07-18, in  for National Mandate Party, AMRAN, S.E.: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction)</t>
         </is>
       </c>
       <c r="M35" t="inlineStr"/>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>16155346930232649735</t>
+          <t>14850548083090834969</t>
         </is>
       </c>
       <c r="J36" t="b">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>M. Nasir: Politician, Nasir Khan: Politician, Nasir Khan: Deceased 1974-05-03</t>
+          <t>M. Nasir: Politician, M. Nasir, male, born 1973-03-19, Nasir Khan: Politician, Nasir Khan Khattak, male, born 1966-02-09, Nasir Khan: Deceased 1974-05-03</t>
         </is>
       </c>
       <c r="M36" t="inlineStr"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>15258324493200127242</t>
+          <t>9575285400559786672</t>
         </is>
       </c>
       <c r="J37" t="b">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Mardani: Politician for Prosperous Justice Party, Mardani Ali Sera: Politician for Prosperous Justice Party, Dr. H. MARDANI, M.Eng.: Public figure: Member of Dewan Perwakilan Rakyat (Prosperous Justice Party Faction)</t>
+          <t>Mardani: Politician, Mardani, born 1968-04-09 for Prosperous Justice Party, Mardani Ali Sera: Politician, Mardani, male, born 1968-04-09, in Jakarta for Prosperous Justice Party, Dr. H. MARDANI, M.Eng.: Public figure: Member of Dewan Perwakilan Rakyat (Prosperous Justice Party Faction)</t>
         </is>
       </c>
       <c r="M37" t="inlineStr"/>
@@ -2393,7 +2393,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>12673510249810812349</t>
+          <t>11352902748996272337</t>
         </is>
       </c>
       <c r="J38" t="b">
@@ -2406,7 +2406,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Muslim: Politician, Muslim: Politician for Democratic Party, MUSLIM, SHI, MM: Public figure: Member of Dewan Perwakilan Rakyat (Democrat Party Faction)</t>
+          <t>Muslim: Politician, Muslim, male, born 1970-08-12, Muslim: Politician, Muslim, male, born 1971-03-01, in  for Democratic Party, MUSLIM, SHI, MM: Public figure: Member of Dewan Perwakilan Rakyat (Democrat Party Faction)</t>
         </is>
       </c>
       <c r="M38" t="inlineStr"/>
@@ -2440,7 +2440,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>3445498252710501515</t>
+          <t>6265423356085323035</t>
         </is>
       </c>
       <c r="J39" t="b">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Nasarudin: Politician for Golongan Karya Party, Nasaruddin: Politician for Great Indonesia Movement Party, Nasrudin: Politician for Golongan Karya Party</t>
+          <t>Nasarudin: Politician, Nasarudin, male, born 1982-07-12 for Golongan Karya Party, Nasaruddin: Politician, Nasaruddin, male, born 1957-07-17 for Great Indonesia Movement Party, Nasrudin: Politician, Nasrudin, male, born 1957-05-24, in Brebes for Golongan Karya Party</t>
         </is>
       </c>
       <c r="M39" t="inlineStr"/>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>8325145406213669318</t>
+          <t>10356402327637780484</t>
         </is>
       </c>
       <c r="J40" t="b">
@@ -2500,7 +2500,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Nasrullah: Politician for National Mandate Party, Mat Solar: Politician for United Development Party</t>
+          <t>Nasrullah: Politician, Nasrullah, male, born 1968-11-18, in Pekalongan for National Mandate Party, Mat Solar: Politician, Nasrullah, male, born 1962-12-04, in Jakarta for United Development Party</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>15437333715055664225</t>
+          <t>7750684464465738003</t>
         </is>
       </c>
       <c r="J41" t="b">
@@ -2560,7 +2560,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Nur'aeni: Politician for Democratic Party, Nuraini: Politician for National Awakening Party, Nuraini: Politician for Indonesian Democratic Party – Struggle</t>
+          <t>Nur'aeni: Politician, Nur'aeni, female, born 1974-10-05 for Democratic Party, Nuraini: Politician, Nuraini, female, born 1989-01-13 for National Awakening Party, Nuraini: Politician, Nuraini, female, born 1973-06-10 for Indonesian Democratic Party – Struggle</t>
         </is>
       </c>
       <c r="M41" t="inlineStr"/>
@@ -2594,7 +2594,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>13506611728240022063</t>
+          <t>6272206608660996122</t>
         </is>
       </c>
       <c r="J42" t="b">
@@ -2607,7 +2607,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Nuraini: Politician for National Awakening Party, Nuraini: Politician for Indonesian Democratic Party – Struggle, Nur'aeni: Politician for Democratic Party</t>
+          <t>Nuraini: Politician, Nuraini, female, born 1989-01-13 for National Awakening Party, Nuraini: Politician, Nuraini, female, born 1973-06-10 for Indonesian Democratic Party – Struggle, Nur'aeni: Politician, Nur'aeni, female, born 1974-10-05 for Democratic Party</t>
         </is>
       </c>
       <c r="M42" t="inlineStr"/>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>9410990259407612881</t>
+          <t>12606550593972603168</t>
         </is>
       </c>
       <c r="J43" t="b">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Nuryati: Politician for Prosperous Justice Party, Nurhayati: Politician for United Development Party, Hj. NURHAYATI: Public figure: Member of Dewan Perwakilan Rakyat (United Development Party Faction)</t>
+          <t>Nuryati: Politician, Nuryati, female, born 1975-03-01 for Prosperous Justice Party, Nurhayati: Politician, Nurhayati, female, born 1969-11-20, in Tasikmalaya for United Development Party, Hj. NURHAYATI: Public figure: Member of Dewan Perwakilan Rakyat (United Development Party Faction)</t>
         </is>
       </c>
       <c r="M43" t="inlineStr"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>16006265390045451114</t>
+          <t>7377647052743484592</t>
         </is>
       </c>
       <c r="J44" t="b">
@@ -2735,7 +2735,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>4217509538874047899</t>
+          <t>489176609753245026</t>
         </is>
       </c>
       <c r="J45" t="b">
@@ -2748,7 +2748,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Amiruddin: Politician for Democratic Party, Amirudin: Politician</t>
+          <t>Amiruddin: Politician, Amiruddin, male, born 1951-11-10 for Democratic Party, Amirudin: Politician, Amirudin, male, born 1971-12-13</t>
         </is>
       </c>
       <c r="M45" t="inlineStr"/>
@@ -2782,7 +2782,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>618597463648689867</t>
+          <t>15310165156767267727</t>
         </is>
       </c>
       <c r="J46" t="b">
@@ -2795,7 +2795,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Usman Khan: Politician for Pakistan Tehreek-e-Insaf, Usmandy S: Politician</t>
+          <t>Usman Khan: Politician, Usman Khan, male, born 1947-09-01, in  for Pakistan Tehreek-e-Insaf, Usmandy S: Politician, Usmandy S, male, born 1966-03-27</t>
         </is>
       </c>
       <c r="M46" t="inlineStr"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>5197650348148788133</t>
+          <t>3044826721493766866</t>
         </is>
       </c>
       <c r="J47" t="b">
@@ -2842,7 +2842,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Muhammad Hamza: Deceased 2021-08-29, T. K. Hamza: Politician for Communist Party of India (Marxist)</t>
+          <t>Muhammad Hamza: Deceased 2021-08-29, T. K. Hamza: Politician, T. K. Hamza, male, born 1937-07-14, in Wandoor for Communist Party of India (Marxist)</t>
         </is>
       </c>
       <c r="M47" t="inlineStr"/>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>5958678241728167086</t>
+          <t>17115703565932051634</t>
         </is>
       </c>
       <c r="J48" t="b">
@@ -2889,7 +2889,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>T. K. Hamza: Politician for Communist Party of India (Marxist), Muhammad Hamza: Deceased 2021-08-29</t>
+          <t>T. K. Hamza: Politician, T. K. Hamza, male, born 1937-07-14, in Wandoor for Communist Party of India (Marxist), Muhammad Hamza: Deceased 2021-08-29</t>
         </is>
       </c>
       <c r="M48" t="inlineStr"/>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>1345752012303240683</t>
+          <t>17671292617135772473</t>
         </is>
       </c>
       <c r="J49" t="b">
@@ -2940,7 +2940,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Usman Ibrahim: Politician for Pakistan Muslim League (N), Usman Ibrahim: Politician for Pakistan Muslim League (N)</t>
+          <t>Usman Ibrahim: Politician, Usman Ibrahim, male, born 1939-09-01, in Gujranwala District for Pakistan Muslim League (N), Usman Ibrahim: Politician, Usman Ibrahim, male, born 1939-09-01, in Gujranwala District for Pakistan Muslim League (N)</t>
         </is>
       </c>
       <c r="M49" t="inlineStr"/>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>7669551443160369142</t>
+          <t>10649917963635957822</t>
         </is>
       </c>
       <c r="J50" t="b">
@@ -2987,7 +2987,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Ilham: Politician, Ilham: Politician</t>
+          <t>Ilham: Politician, Ilham, male, born 1968-09-08, Ilham: Politician, Ilham, male, born 1975-05-08</t>
         </is>
       </c>
       <c r="M50" t="inlineStr"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>13812526029936423970</t>
+          <t>11514338939174168986</t>
         </is>
       </c>
       <c r="J51" t="b">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>A. R. Iwansyah: Politician, Iwansyah: Politician</t>
+          <t>A. R. Iwansyah: Politician, A. R. Iwansyah, male, born 1960-08-11, Iwansyah: Politician, Iwansyah, male, born 1959-07-09</t>
         </is>
       </c>
       <c r="M51" t="inlineStr"/>
@@ -3068,7 +3068,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>14612635024796745373</t>
+          <t>3786715363206398007</t>
         </is>
       </c>
       <c r="J52" t="b">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Mohammad Ali Jafari Brigadier Commander: Not an Indonesian name: محمد علي جعفري, Sayed Jafar: Politician</t>
+          <t>Mohammad Ali Jafari Brigadier Commander: Not an Indonesian name: محمد علي جعفري, Sayed Jafar: Politician, Sayed Jafar, male, born 1962-03-17</t>
         </is>
       </c>
       <c r="M52" t="inlineStr"/>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>7488243478192424675</t>
+          <t>15937969915934630320</t>
         </is>
       </c>
       <c r="J53" t="b">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Ali Barakat: Not an Indonesian name: علي بركات, Ali: Politician</t>
+          <t>Ali Barakat: Not an Indonesian name: علي بركات, Ali: Politician, Ali, male, born 1950-09-01</t>
         </is>
       </c>
       <c r="M53" t="inlineStr"/>
@@ -3170,7 +3170,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>15438446431812825139</t>
+          <t>18003503116651270547</t>
         </is>
       </c>
       <c r="J54" t="b">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>'Abd al-Rahman Khalaf 'Ubayd Juday' AL-'ANIZI: 'Abd al-Rahman Khalaf AL-'ANZI, AL-RAHMAN, Abu Usamah, ABU USAMA, YUSUF, 'Abd al-Rahman Khalaf AL-ANIZI, KUWAITI, Abu Shaima', AL-KUWAITI, Abu Usamah</t>
+          <t>'Abd al-Rahman Khalaf 'Ubayd Juday' AL-'ANIZI: 'Abd al-Rahman Khalaf AL-'ANZI, AL-RAHMAN, Abu Usamah, ABU USAMA, YUSUF, 'Abd al-Rahman Khalaf AL-ANIZI, KUWAITI, Abu Shaima', AL-KUWAITI, Abu Usamah, born 01 Jan 1973 to 31 Dec 1973</t>
         </is>
       </c>
     </row>
@@ -3221,7 +3221,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>7707983577647246311</t>
+          <t>11655220696173397919</t>
         </is>
       </c>
       <c r="J55" t="b">
@@ -3234,7 +3234,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Amin Ak: Politician for Prosperous Justice Party, M. Amin: Politician</t>
+          <t>Amin Ak: Politician, Amin, male, born 1965-07-06 for Prosperous Justice Party, M. Amin: Politician, M. Amin, male, born 1965-09-26</t>
         </is>
       </c>
       <c r="M55" t="inlineStr"/>
@@ -3268,7 +3268,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>13090590572403068824</t>
+          <t>3913189880287947192</t>
         </is>
       </c>
       <c r="J56" t="b">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Kh. M. Mansyur: Politician, Mansour Fadlallah Azzam: Not an Indonesian name: منصور فضل الله عزام</t>
+          <t>Kh. M. Mansyur: Politician, Kh. M. Mansyur, male, born 1947-06-10, Mansour Fadlallah Azzam: Not an Indonesian name: منصور فضل الله عزام</t>
         </is>
       </c>
       <c r="M56" t="inlineStr"/>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>11117354032143609104</t>
+          <t>4810521403310891072</t>
         </is>
       </c>
       <c r="J57" t="b">
@@ -3328,7 +3328,7 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Nurhasanah: Politician for Democratic Party, Norhasanah: Politician for United Development Party</t>
+          <t>Nurhasanah: Politician, Nurhasanah, female, born 1957-02-22 for Democratic Party, Norhasanah: Politician, Norhasanah, female, born 1962-11-09, in Martapura for United Development Party</t>
         </is>
       </c>
       <c r="M57" t="inlineStr"/>
@@ -3362,7 +3362,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>5542636466266035152</t>
+          <t>3533842459388614228</t>
         </is>
       </c>
       <c r="J58" t="b">
@@ -3375,7 +3375,7 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Salahudin: Politician, Sheikh Salahuddin: Politician for Muttahida Qaumi Movement</t>
+          <t>Salahudin: Politician, Salahudin, male, born 1969-10-12, Sheikh Salahuddin: Politician, Sheikh Salahuddin, male, born 1956-08-20 for Muttahida Qaumi Movement</t>
         </is>
       </c>
       <c r="M58" t="inlineStr"/>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>10574175479781187770</t>
+          <t>3768594917827469901</t>
         </is>
       </c>
       <c r="J59" t="b">
@@ -3422,7 +3422,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Syamsurizal: Politician for United Development Party, Samsuri: Politician</t>
+          <t>Syamsurizal: Politician, Syamsurizal, male, born 1955-06-25 for United Development Party, Samsuri: Politician, Samsuri, male, born 1952-04-20</t>
         </is>
       </c>
       <c r="M59" t="inlineStr"/>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>9049477210193472028</t>
+          <t>14922391628114781910</t>
         </is>
       </c>
       <c r="J60" t="b">
@@ -3469,7 +3469,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Muhammad Syarifuddin: Politician, Syarifuddin: Politician</t>
+          <t>Muhammad Syarifuddin: Politician, M. Syarifuddin, male, born 1954-10-17, in Baturaja, Syarifuddin: Politician, Syarifuddin, male, born 1965-10-19</t>
         </is>
       </c>
       <c r="M60" t="inlineStr"/>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>1653152577468124225</t>
+          <t>16976888617006172996</t>
         </is>
       </c>
       <c r="J61" t="b">
@@ -3520,7 +3520,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Siti Nurbaya Bakar: Politician for Nasdem Party, SITI Nurbaya Bakar: Public figure: Min. of Environment &amp; Forestry</t>
+          <t>Siti Nurbaya Bakar: Politician, Siti Nurbaya, Dr. Ir. Siti Nurbaya Bakar, M.Sc., female, born 1956-08-28, in Jakarta for Nasdem Party, SITI Nurbaya Bakar: Public figure: Min. of Environment &amp; Forestry</t>
         </is>
       </c>
       <c r="M61" t="inlineStr"/>
@@ -3558,7 +3558,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>11796289968786095693</t>
+          <t>8835002230478851975</t>
         </is>
       </c>
       <c r="J62" t="b">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Siti Nurbaya Bakar: Politician for Nasdem Party, SITI Nurbaya Bakar: Public figure: Min. of Environment &amp; Forestry</t>
+          <t>Siti Nurbaya Bakar: Politician, Siti Nurbaya, Dr. Ir. Siti Nurbaya Bakar, M.Sc., female, born 1956-08-28, in Jakarta for Nasdem Party, SITI Nurbaya Bakar: Public figure: Min. of Environment &amp; Forestry</t>
         </is>
       </c>
       <c r="M62" t="inlineStr"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>16809459174214547971</t>
+          <t>11660482386343856849</t>
         </is>
       </c>
       <c r="J63" t="b">
@@ -3622,7 +3622,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Siti Nurbaya Bakar: Politician for Nasdem Party, SITI Nurbaya Bakar: Public figure: Min. of Environment &amp; Forestry</t>
+          <t>Siti Nurbaya Bakar: Politician, Siti Nurbaya, Dr. Ir. Siti Nurbaya Bakar, M.Sc., female, born 1956-08-28, in Jakarta for Nasdem Party, SITI Nurbaya Bakar: Public figure: Min. of Environment &amp; Forestry</t>
         </is>
       </c>
       <c r="M63" t="inlineStr"/>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>4048053608589769034</t>
+          <t>2886418286232450298</t>
         </is>
       </c>
       <c r="J64" t="b">
@@ -3703,7 +3703,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>982755505615538247</t>
+          <t>11518251025373546980</t>
         </is>
       </c>
       <c r="J65" t="b">
@@ -3716,7 +3716,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Sunardi: Politician for Prosperous Justice Party, Sunardi: Politician</t>
+          <t>Sunardi: Politician, Sunardi, male, born 1966-12-05 for Prosperous Justice Party, Sunardi: Politician, Sunardi, male, born 1948-02-09</t>
         </is>
       </c>
       <c r="M65" t="inlineStr"/>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>16998896165995472831</t>
+          <t>18174297855659911712</t>
         </is>
       </c>
       <c r="J66" t="b">
@@ -3763,7 +3763,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Supratman: Politician for Indonesian Justice and Unity Party, Supratman: Politician</t>
+          <t>Supratman: Politician, Supratman, male, born 1959-05-04, in Medan for Indonesian Justice and Unity Party, Supratman: Politician, Supratman, male, born 1949-10-05</t>
         </is>
       </c>
       <c r="M66" t="inlineStr"/>
@@ -3797,7 +3797,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>3448517967846851818</t>
+          <t>17481581452213201151</t>
         </is>
       </c>
       <c r="J67" t="b">
@@ -3810,7 +3810,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Supriadi: Politician, Supriadi: Politician</t>
+          <t>Supriadi: Politician, Supriadi, male, born 1968-08-08, Supriadi: Politician, Supriadi, male, born 1968-01-04</t>
         </is>
       </c>
       <c r="M67" t="inlineStr"/>
@@ -3844,7 +3844,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>3408243776120140158</t>
+          <t>7918233431691663956</t>
         </is>
       </c>
       <c r="J68" t="b">
@@ -3857,7 +3857,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Syafrudin: Politician for Nasdem Party, Syafruddin: Politician</t>
+          <t>Syafrudin: Politician, Syafrudin, male, born 1958-08-10 for Nasdem Party, Syafruddin: Politician, Syafruddin, male, born 1958-07-20</t>
         </is>
       </c>
       <c r="M68" t="inlineStr"/>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>9248070174289797635</t>
+          <t>17727646768577443087</t>
         </is>
       </c>
       <c r="J69" t="b">
@@ -3904,7 +3904,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Syamsurizal: Politician for United Development Party, Samsuri: Politician</t>
+          <t>Syamsurizal: Politician, Syamsurizal, male, born 1955-06-25 for United Development Party, Samsuri: Politician, Samsuri, male, born 1952-04-20</t>
         </is>
       </c>
       <c r="M69" t="inlineStr"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>4986779605688232716</t>
+          <t>14514591989024359005</t>
         </is>
       </c>
       <c r="J70" t="b">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Usman Khan: Politician for Pakistan Tehreek-e-Insaf, Usmandy S: Politician</t>
+          <t>Usman Khan: Politician, Usman Khan, male, born 1947-09-01, in  for Pakistan Tehreek-e-Insaf, Usmandy S: Politician, Usmandy S, male, born 1966-03-27</t>
         </is>
       </c>
       <c r="M70" t="inlineStr"/>
@@ -3985,7 +3985,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>7327461934733985848</t>
+          <t>10166813688394463510</t>
         </is>
       </c>
       <c r="J71" t="b">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Amin Ak: Politician for Prosperous Justice Party, M. Amin: Politician</t>
+          <t>Amin Ak: Politician, Amin, male, born 1965-07-06 for Prosperous Justice Party, M. Amin: Politician, M. Amin, male, born 1965-09-26</t>
         </is>
       </c>
       <c r="M71" t="inlineStr"/>

</xml_diff>

<commit_message>
Allow output to be .csv
branch:
</commit_message>
<xml_diff>
--- a/tests/test_resources/test_namescan/test_namescan-explained.xlsx
+++ b/tests/test_resources/test_namescan/test_namescan-explained.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4558967249527932496</t>
+          <t>10690394630159179216</t>
         </is>
       </c>
       <c r="J2" t="b">
@@ -594,7 +594,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>9081041506290180432</t>
+          <t>8383772502347693165</t>
         </is>
       </c>
       <c r="J3" t="b">
@@ -645,7 +645,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>7394138728020829710</t>
+          <t>12713458539162444596</t>
         </is>
       </c>
       <c r="J4" t="b">
@@ -705,7 +705,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>13477009712307192955</t>
+          <t>17183571439025306501</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -771,7 +771,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>17777211603270557273</t>
+          <t>16291883044465602181</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -827,7 +827,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>9345809663888044064</t>
+          <t>1004739815597641664</t>
         </is>
       </c>
       <c r="J7" t="b">
@@ -874,7 +874,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>16787390437967957881</t>
+          <t>14132829364961678458</t>
         </is>
       </c>
       <c r="J8" t="b">
@@ -925,7 +925,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2993838869014342318</t>
+          <t>15814197177705055138</t>
         </is>
       </c>
       <c r="J9" t="b">
@@ -972,7 +972,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>6576989606114601390</t>
+          <t>17153322923920234955</t>
         </is>
       </c>
       <c r="J10" t="b">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>4836203185392951978</t>
+          <t>16349991511598102228</t>
         </is>
       </c>
       <c r="J11" t="b">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>8761211111575463348</t>
+          <t>2480747059259408109</t>
         </is>
       </c>
       <c r="J12" t="b">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>6813420260146292579</t>
+          <t>15329413453490575982</t>
         </is>
       </c>
       <c r="J13" t="b">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>6488034680104985054</t>
+          <t>7877352591372251384</t>
         </is>
       </c>
       <c r="J14" t="b">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>7761883952758496458</t>
+          <t>2359784791348081432</t>
         </is>
       </c>
       <c r="J15" t="b">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>8365530065398086069</t>
+          <t>9921084047202697485</t>
         </is>
       </c>
       <c r="J16" t="b">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>208773953576434720</t>
+          <t>15106319062049085917</t>
         </is>
       </c>
       <c r="J17" t="b">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>14958980638395977557</t>
+          <t>17887618648411249842</t>
         </is>
       </c>
       <c r="J18" t="b">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>10592543599469362806</t>
+          <t>1968137505995152539</t>
         </is>
       </c>
       <c r="J19" t="b">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>5443673151062899518</t>
+          <t>15537643808888923564</t>
         </is>
       </c>
       <c r="J20" t="b">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>14630247723957871873</t>
+          <t>8962903224833921675</t>
         </is>
       </c>
       <c r="J21" t="b">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>6618276129218788492</t>
+          <t>17839782897218791783</t>
         </is>
       </c>
       <c r="J22" t="b">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>14266958555859629077</t>
+          <t>11449381584423265720</t>
         </is>
       </c>
       <c r="J23" t="b">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>12972531040749141575</t>
+          <t>10265562418216162887</t>
         </is>
       </c>
       <c r="J24" t="b">
@@ -1756,7 +1756,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>11869132067293909402</t>
+          <t>5421264852785133268</t>
         </is>
       </c>
       <c r="J25" t="b">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>7066761180596573176</t>
+          <t>9775940493315330056</t>
         </is>
       </c>
       <c r="J26" t="b">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>11690031790147095061</t>
+          <t>657157722172498361</t>
         </is>
       </c>
       <c r="J27" t="b">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>12182520774192383997</t>
+          <t>13865823427859795782</t>
         </is>
       </c>
       <c r="J28" t="b">
@@ -1950,7 +1950,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>6552148137850177530</t>
+          <t>4032755431706838771</t>
         </is>
       </c>
       <c r="J29" t="b">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>17672577618118732994</t>
+          <t>17232621134687114681</t>
         </is>
       </c>
       <c r="J30" t="b">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>13934406406176155609</t>
+          <t>16341410120344876481</t>
         </is>
       </c>
       <c r="J31" t="b">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>8830964935097315160</t>
+          <t>5907976161846496194</t>
         </is>
       </c>
       <c r="J32" t="b">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>6546123067562796969</t>
+          <t>7975738456852880511</t>
         </is>
       </c>
       <c r="J33" t="b">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>811237689581992791</t>
+          <t>9926735972810321660</t>
         </is>
       </c>
       <c r="J34" t="b">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>16141970136513248035</t>
+          <t>11896088144577639464</t>
         </is>
       </c>
       <c r="J35" t="b">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>14850548083090834969</t>
+          <t>3608772417383295319</t>
         </is>
       </c>
       <c r="J36" t="b">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>9575285400559786672</t>
+          <t>16143978711353994814</t>
         </is>
       </c>
       <c r="J37" t="b">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>11352902748996272337</t>
+          <t>14042058008958797846</t>
         </is>
       </c>
       <c r="J38" t="b">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>6265423356085323035</t>
+          <t>7569868334157635296</t>
         </is>
       </c>
       <c r="J39" t="b">
@@ -2487,7 +2487,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>10356402327637780484</t>
+          <t>9099142108530947764</t>
         </is>
       </c>
       <c r="J40" t="b">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>7750684464465738003</t>
+          <t>13654721657899965579</t>
         </is>
       </c>
       <c r="J41" t="b">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>6272206608660996122</t>
+          <t>15390026578503934594</t>
         </is>
       </c>
       <c r="J42" t="b">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>12606550593972603168</t>
+          <t>5628284592660666110</t>
         </is>
       </c>
       <c r="J43" t="b">
@@ -2688,7 +2688,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>7377647052743484592</t>
+          <t>7051504758948289199</t>
         </is>
       </c>
       <c r="J44" t="b">
@@ -2735,7 +2735,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>489176609753245026</t>
+          <t>13907261259539446977</t>
         </is>
       </c>
       <c r="J45" t="b">
@@ -2782,7 +2782,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>15310165156767267727</t>
+          <t>13643525414110346129</t>
         </is>
       </c>
       <c r="J46" t="b">
@@ -2829,7 +2829,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>3044826721493766866</t>
+          <t>1075559904491387889</t>
         </is>
       </c>
       <c r="J47" t="b">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>17115703565932051634</t>
+          <t>4096567415949925093</t>
         </is>
       </c>
       <c r="J48" t="b">
@@ -2927,7 +2927,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>17671292617135772473</t>
+          <t>17630198932028886607</t>
         </is>
       </c>
       <c r="J49" t="b">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>10649917963635957822</t>
+          <t>2294922347497119376</t>
         </is>
       </c>
       <c r="J50" t="b">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>11514338939174168986</t>
+          <t>1423331922884228284</t>
         </is>
       </c>
       <c r="J51" t="b">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>3786715363206398007</t>
+          <t>10615855276681504905</t>
         </is>
       </c>
       <c r="J52" t="b">
@@ -3119,7 +3119,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>15937969915934630320</t>
+          <t>2138890619822242194</t>
         </is>
       </c>
       <c r="J53" t="b">
@@ -3170,7 +3170,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>18003503116651270547</t>
+          <t>12410837511217930970</t>
         </is>
       </c>
       <c r="J54" t="b">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>11655220696173397919</t>
+          <t>4922484447229694772</t>
         </is>
       </c>
       <c r="J55" t="b">
@@ -3268,7 +3268,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>3913189880287947192</t>
+          <t>9952986022782453851</t>
         </is>
       </c>
       <c r="J56" t="b">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>4810521403310891072</t>
+          <t>15752068823501477755</t>
         </is>
       </c>
       <c r="J57" t="b">
@@ -3362,7 +3362,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>3533842459388614228</t>
+          <t>17942581698056827285</t>
         </is>
       </c>
       <c r="J58" t="b">
@@ -3409,7 +3409,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>3768594917827469901</t>
+          <t>14101280709920695794</t>
         </is>
       </c>
       <c r="J59" t="b">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>14922391628114781910</t>
+          <t>12074244793306088426</t>
         </is>
       </c>
       <c r="J60" t="b">
@@ -3507,7 +3507,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>16976888617006172996</t>
+          <t>10198157551146233134</t>
         </is>
       </c>
       <c r="J61" t="b">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>8835002230478851975</t>
+          <t>14148964815780679069</t>
         </is>
       </c>
       <c r="J62" t="b">
@@ -3609,7 +3609,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>11660482386343856849</t>
+          <t>15941531297468623633</t>
         </is>
       </c>
       <c r="J63" t="b">
@@ -3656,7 +3656,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>2886418286232450298</t>
+          <t>2864936459970274854</t>
         </is>
       </c>
       <c r="J64" t="b">
@@ -3703,7 +3703,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>11518251025373546980</t>
+          <t>12329970119364176493</t>
         </is>
       </c>
       <c r="J65" t="b">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>18174297855659911712</t>
+          <t>15005498962532913587</t>
         </is>
       </c>
       <c r="J66" t="b">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>17481581452213201151</t>
+          <t>3334340575287454550</t>
         </is>
       </c>
       <c r="J67" t="b">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>7918233431691663956</t>
+          <t>6565147969932097068</t>
         </is>
       </c>
       <c r="J68" t="b">
@@ -3891,7 +3891,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>17727646768577443087</t>
+          <t>12047674144465933605</t>
         </is>
       </c>
       <c r="J69" t="b">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>14514591989024359005</t>
+          <t>13777818520146174391</t>
         </is>
       </c>
       <c r="J70" t="b">
@@ -3985,7 +3985,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>10166813688394463510</t>
+          <t>5590615921804060233</t>
         </is>
       </c>
       <c r="J71" t="b">

</xml_diff>

<commit_message>
Upgrade to namescan v3
which emits camel case JSON

branch:
</commit_message>
<xml_diff>
--- a/tests/test_resources/test_namescan/test_namescan-explained.xlsx
+++ b/tests/test_resources/test_namescan/test_namescan-explained.xlsx
@@ -541,27 +541,25 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Muhammad Ali DURGHAM: Not an Indonesian name: محمد علي, Muhammad Yousuf Ali: Deceased 1998, Muhammad Rapsel Ali: Politician, Muhammad Rapsel Ali, male, born 1971-05-06 for Nasdem Party, Ali Nasir Muhammad: Not an Indonesian name: علي ناصر محمد, Muhammad Yusuf Ali: Deceased 1998-12-01, Muhammad Ali Ridha: Politician, Muhammad Ali Ridha, male, born 1971-02-04 for Golongan Karya Party, Muhammad Ali Malkani: Politician, Muhammad Ali Malkani, male, born 1966-11-22 for Pakistan Peoples Party, Muhammad Ali DURGHAM: Not an Indonesian name: محمد علي, Mohammed Ali NASR: Not an Indonesian name: محمد علي نصر, Mohammed Ali NASR: Not an Indonesian name: محمد علي نصر, Muhammad Shujat Ali: Deceased 2007-04-01, Mohammad Ali JAFARI: Not an Indonesian name: محمد علي جعفري, Iqbal Muhammad Ali Khan: Deceased 2022-04-19, Malek ALI: Suspect in Syrian conflict, Akram Muhammad AL-SALTI: Public figure: Commander-in-Chief and Chief of Staff of the Palestine Liberation Army, Muhammad AL-QATIRJI: Suspect in Syrian conflict, Muhammad Alwi Dahlan: Politician, Muhammad Alwi Dahlan, male, born 1933-05-15, in Padang, Muhammad Rudini Darwan Ali: Politician, Muhammad Rudini Darwan Ali, male, born 1986-05-09, Muhammad Unais Ali Hisyam: Politician, Muhammad Unais Ali Hisyam, male, born 1973-12-14, in , Habib Muhammad Ali Al'habsyi: Politician, Habib Muhammad Ali Al'habsyi, male, born 1969-07-16, Mohammad Ali Shah: Deceased 2013-02-04, K.H. MUH. UNAIS ALI HISYAM, M.Pd.I: Public figure: Member of Dewan Perwakilan Rakyat (National Awakening Party Faction), Muhammad Ibrahim al-Shaar: Suspect in Syrian conflict, ALI KONY: Public figure: Deputy, Lord’s Resistance Army, Mohammad Ali Jinnah: Deceased 1948-09-11, Husayn Muhamad Husayn al-Juaythini: Foreigner: PALESTINIAN TERRITORY, Occupied, Mohammadian Abbas-Ali: Not an Indonesian name: Мохаммадян Аббас-Али, Ali Ahsan Mohammad Mojaheed: Deceased 2015-11-22, Mohammad Ali ZANJIREI: Public figure: Senior advisor to Head and Deputy Head of Iran's Prisons Organisation, Mohammad Ali JAFARI: Public figure: Former Commander of the IRGC. Currently head of the Hazrat Baqiatollah al-Azam Cultural and Social 
-Headquarters., Mohammad Ali JAFARI: Public figure: Former Commander of the IRGC. Currently head of the Hazrat Baqiatollah al-Azam Cultural and Social 
-Headquarters.</t>
+          <t>Mohammed Ali NASR: Not an Indonesian name: محمد علي نصر, Muhammad Ali Malkani: Politician, Muhammad Ali Malkani, male, born 1966-11-22 for Pakistan Peoples Party, Ali Nasir Muhammad: Not an Indonesian name: علي ناصر محمد, Muhammad Rapsel Ali: Politician, Muhammad Rapsel Ali, male, born 1971-05-06 for Nasdem Party, Muhammad Shujat Ali: Deceased 2007-04-01, Muhammad Yousuf Ali: Deceased 1998, Muhammad Ali Ridha: Politician, Muhammad Ali Ridha, male, born 1971-02-04 for Golongan Karya Party, Mohammed Ali NASR: Not an Indonesian name: محمد علي نصر, Muhammad Ali DURGHAM: Not an Indonesian name: محمد علي, Muhammad Ali DURGHAM: Not an Indonesian name: محمد علي, Muhammad Yusuf Ali: Deceased 1998-12-01, Iqbal Muhammad Ali Khan: Deceased 2022-04-19, Muhammad Alwi Dahlan: Politician, Muhammad Alwi Dahlan, male, born 1933-05-15, in Padang, Muhammad Unais Ali Hisyam: Politician, Muhammad Unais Ali Hisyam, male, born 1973-12-14, in , Muhammad Rudini Darwan Ali: Politician, Muhammad Rudini Darwan Ali, male, born 1986-05-09, Mohammad Ali Shah: Deceased 2013-02-04, Habib Muhammad Ali Al'habsyi: Politician, Habib Muhammad Ali Al'habsyi, male, born 1969-07-16, K.H. MUH. UNAIS ALI HISYAM, M.Pd.I: Public figure: Member of Dewan Perwakilan Rakyat (National Awakening Party Faction), Mohammad Ali JAFARI: Not an Indonesian name: محمد علي جعفري, Mohammad Ali Jinnah: Deceased 1948-09-11, ALI KONY: Public figure: Deputy, Lord’s Resistance Army, Mohammadian Abbas-Ali: Not an Indonesian name: Мохаммадян Аббас-Али, Abbas-Ali Mohammadian: Not an Indonesian name: عباسعلی محمدیان, Hodjatoleslam Ali KHAN MOHAMMADI: Not an Indonesian name: حجت الاسلام علی خان محمدی, Abbas-Ali MOHAMMADIAN: Not an Indonesian name: محمدیان عباس-علی, Ali Ahsan Mohammad Mojaheed: Deceased 2015-11-22</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Ali Kony: Ali Kony is a Deputy in the Lord's Resistance Army (LRA) (CFe.002), a designated entity and the son of LRA leader Joseph Kony (CFi.009), a designated individual. Ali was incorporated into the LRA's leadership hierarchy in 2010.  He is part of a group of senior LRA officers who are based with Joseph Kony., Kony Ali: Sanctions: art. 2, para. 1 let. a (Financial sanctions) et art. 4, para. 1 (Travel ban)
+          <t>Ali Kony: Ali Kony is a Deputy in the Lord's Resistance Army (LRA) (CFe.002), a designated entity and the son of LRA leader Joseph Kony (CFi.009), a designated individual. Ali was incorporated into the LRA's leadership hierarchy in 2010.  He is part of a group of senior LRA officers who are based with Joseph Kony., Jafari Mohammad Ali: Foreign identifier: 28.
+Justification: Former Commander of the IRGC. Currently head of the Hazrat Baqiatollah al-Azam Cultural and Social Headquarters.
+Sanctions: Art. 7 Abs. 1 (Finanzsanktionen), Art. 10 Abs. 1 und 3 (Ein- und Durchreiseverbot) und Art. 11 Bst. b (Verbot der Erfüllung bestimmter Forderungen), Anhang 6, Ramin Mohammad-Ali: Foreign identifier: 68.
+Justification: Secretary-general of the World Holocaust Foundation, established at the International Conference to Review the Global Vision of the Holocaust in 2006, which Ramin was responsible for organising on behalf of the Iranian Government. Main figure responsible for censorship as Vice-Minister in charge of the Press up to Dec 2013, being directly responsible for the closure of many reforming newspapers (Etemad, Etemad-e Melli, Shargh, etc), closure of the Independent Press Syndicate and the intimidation or arrest of journalists.
+Sanctions: Art. 7 Abs. 1 (Finanzsanktionen) und Art. 11 Bst. b (Verbot der Erfüllung bestimmter Forderungen), Anhang 7, Zanjirei Mohammad-Ali: Foreign identifier: 32.
+Justification: As Senior advisor to Head, and Deputy Head of Iran's Prisons Organisation, responsible for serious human rights violations against prisoners. Administered a system in which prisoners suffered abuse, torture and inhuman/degrading treatment and were accommodated in very poor living conditions.
+Sanctions: Art. 7 Abs. 1 (Finanzsanktionen) und Art. 11 Bst. b (Verbot der Erfüllung bestimmter Forderungen), Anhang 7, Jafari Mohammad-Ali: Foreign identifier: 6.
+Justification: Director of the Hazrat-e Baqiatollah Social and Cultural Base. Former Commander of the IRGC (Sep 2007 - Apr 2019). IRGC and the Sarollah Base commanded by General Mohammad-Ali (Aziz) Jafari have played a key role in illegally interfering with the 2009 Presidential Elections, arresting and detaining political activists, as well as clashing with protestors in the streets.
+Sanctions: Art. 7 Abs. 1 (Finanzsanktionen) und Art. 11 Bst. b (Verbot der Erfüllung bestimmter Forderungen), Anhang 7, Kony Ali: Sanctions: Art. 2 Abs. 1 Bst. a (Finanzsanktionen) und 4 Abs. 1 (Ein- und Durchreiseverbot)
 Listed: 2016-08-23
 Other information: Designation: Deputy, Lord’s Resistance Army
-Ali Kony is a deputy in the Lord’s Resistance Army (LRA) (SSID 300-34021), a designated entity and the son of LRA leader Joseph Kony (SSID 300-3976), a designated individual. Ali was incorporated into the LRA’s leadership hierarchy in 2010. He is part of a group of senior LRA officers who are based with Joseph Kony., Jafari Mohammad-Ali: Foreign identifier: 6.
-Justification: Director of the Hazrat-e Baqiatollah Social and Cultural Base. Former Commander of the IRGC (Sep 2007 - Apr 2019). IRGC and the Sarollah Base commanded by General Mohammad-Ali (Aziz) Jafari have played a key role in illegally interfering with the 2009 Presidential Elections, arresting and detaining political activists, as well as clashing with protestors in the streets.
-Sanctions: art. 7 (Financial sanctions) and art. 11 (Prohibition to honour certain claims), annex 7, Ramin Mohammad-Ali: Foreign identifier: 68.
-Justification: Secretary-general of the World Holocaust Foundation, established at the International Conference to Review the Global Vision of the Holocaust in 2006, which Ramin was responsible for organising on behalf of the Iranian Government. Main figure responsible for censorship as Vice-Minister in charge of the Press up to Dec 2013, being directly responsible for the closure of many reforming newspapers (Etemad, Etemad-e Melli, Shargh, etc), closure of the Independent Press Syndicate and the intimidation or arrest of journalists.
-Sanctions: art. 7 (Financial sanctions) and art. 11 (Prohibition to honour certain claims), annex 7, Zanjirei Mohammad-Ali: Foreign identifier: 32.
-Justification: As Senior advisor to Head, and Deputy Head of Iran's Prisons Organisation, responsible for serious human rights violations against prisoners. Administered a system in which prisoners suffered abuse, torture and inhuman/degrading treatment and were accommodated in very poor living conditions.
-Sanctions: art. 7 (Financial sanctions) and art. 11 (Prohibition to honour certain claims), annex 7, Anwar Mohammed ZBOUN: Anwar Muhammad AL-ZBOUN, born 1968, in , Jafari Mohammad Ali: Foreign identifier: 28.
-Justification: Former Commander of the IRGC. Currently head of the Hazrat Baqiatollah al-Azam Cultural and Social Headquarters.
-Sanctions: art. 7 (Financial sanctions), art. 10 (Travel ban) and art. 11 (Prohibition to honour certain claims), annex 6, ALI KHANAMAN MOHAMMADI: Effective Date:05/04/2016; Expiration Date:08/25/2025; Standard Order:Y; Action:FR NOTICE ADDED; FR Citation:81.F.R. 28822 5/10/2016; , Houej Mohamad Ali: Justification: Minister for Industry, Economy and Trade in Colonel Qadhafi's Government. Closely associated with the former regime of Muammar Qadhafi.
-Sanctions: article 2 paragraph 1 (Financial sanctions), annex 3 (part A: individuals, part B: entities and organizations), Houej Mohamad Ali: Justification: Minister for Industry, Economy and Trade in Colonel Qadhafi’s Government. Closely associated with the former regime of Muammar Qadhafi.
-Sanctions: art. 4 (Travel ban), annex 5, Mohamad Ali HOUEJ: Minister for Industry, Economy and Trade in Muammar Qadhafi’s Government., Amr ARMANAZI: Amr Muhammad Najib AL-ARMANAZI, Amr Najib ARMANAZI, born 07 Feb 1944, Mohammadreza Ali AKBARI: (Linked To: QASEMI, Rostam)</t>
+Ali Kony is a deputy in the Lord’s Resistance Army (LRA) (SSID 300-34021), a designated entity and the son of LRA leader Joseph Kony (SSID 300-3976), a designated individual. Ali was incorporated into the LRA’s leadership hierarchy in 2010. He is part of a group of senior LRA officers who are based with Joseph Kony., ALI KHANAMAN MOHAMMADI: Effective Date:05/04/2016; Expiration Date:08/25/2025; Standard Order:Y; Action:FR NOTICE ADDED; FR Citation:81.F.R. 28822 5/10/2016; , Houej Mohamad Ali: Justification: Minister for Industry, Economy and Trade in Colonel Qadhafi's Government. Closely associated with the former regime of Muammar Qadhafi.
+Sanctions: Art. 2 Abs. 1 (Finanzsanktionen), Anhang 3 (Teil A: natürliche Personen, Teil B: Unternehmen und Organisationen), Houej Mohamad Ali: Justification: Minister for Industry, Economy and Trade in Colonel Qadhafi’s Government. Closely associated with the former regime of Muammar Qadhafi.
+Sanctions: Art. 4 (Ein- und Durchreiseverbot), Anhang 5, Mohamad Ali HOUEJ: Minister for Industry, Economy and Trade in Muammar Qadhafi’s Government., Mohammadreza Ali AKBARI: (Linked To: QASEMI, Rostam)</t>
         </is>
       </c>
     </row>
@@ -607,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Mohammad Yahiya Moalla Dr.: Not an Indonesian name: محمد يحيى معلا, Amr Armanazi: Suspect in Syrian conflict, Ahmad Ballul: Not an Indonesian name: أحمد بالول, Mohammad Mufleh: Not an Indonesian name: محمد مفلح, Imad Mohammad Deeb Khamis: Not an Indonesian name: عماد محمد ديب خميس, Mohammed Bilal Brigadier General: Suspect in Syrian conflict, Mohammed Ali Nasr General: Not an Indonesian name: محمد علي نصر, Mohammad Abdul-Sattar Al Sayed Dr.: Not an Indonesian name: محمد عبد الستار السيد, S. Muhammad: Politician, S. Muhammad, male, born 1960-04-25, in Gresik for National Awakening Party, Muhammed Zamrini Brigadier-General: Not an Indonesian name: محمد زمريني, Muhamad: Politician, Muhamad, male, born 1964-04-06, Muhammadong: Politician, Muhammadong, male, born 1969-01-09 for Great Indonesia Movement Party, Muhammad Yousef Hasouri Brigadier General: Not an Indonesian name: محمد يوسف حاصوري, Mohamed Maaruf Brigadier General: Not an Indonesian name: محمد معروف, Mohamad Ghazi Jalali: Suspect in Syrian conflict, Jihad Mohamed Sultan Brigadier General: Not an Indonesian name: جهاد محمد سلطان, Mohamed Khaddor Major General: Not an Indonesian name: محمد خضور, Muhammad Ali Durgham Major General: Not an Indonesian name: محمد علي, Mohammed Jabir: Not an Indonesian name: محمد جابر, Mohamed Heikmat Ibrahim: Not an Indonesian name: محمد حكمت إبراهيم, Mohamad Fayez Barcha: Not an Indonesian name: محمد فايز برشة, Mohamad Amer Mardini: Suspect in Syrian conflict, MuhammadAriLaw: Politician, Muhammad Ari Pratomo, male, born 1982-06-21</t>
+          <t>Mohammed Bilal Brigadier General: Suspect in Syrian conflict, Mohammad Mufleh: Not an Indonesian name: محمد مفلح, Imad Mohammad Deeb Khamis: Not an Indonesian name: عماد محمد ديب خميس, Mohammad Abdul-Sattar Al Sayed Dr.: Not an Indonesian name: محمد عبد الستار السيد, Ahmad Ballul: Not an Indonesian name: أحمد بالول, Mohammed Ali Nasr General: Not an Indonesian name: محمد علي نصر, Amr Armanazi: Suspect in Syrian conflict, Mohammad Yahiya Moalla Dr.: Not an Indonesian name: محمد يحيى معلا, S. Muhammad: Politician, S. Muhammad, male, born 1960-04-25, in Gresik for National Awakening Party, Muhammed Zamrini Brigadier-General: Not an Indonesian name: محمد زمريني, Muhamad: Politician, Muhamad, male, born 1964-04-06, Muhammadong: Politician, Muhammadong, male, born 1969-01-09 for Great Indonesia Movement Party, Muhammad Yousef Hasouri Brigadier General: Not an Indonesian name: محمد يوسف حاصوري, Mohamad Ghazi Jalali: Suspect in Syrian conflict, Mohamed Heikmat Ibrahim: Not an Indonesian name: محمد حكمت إبراهيم, Mohamad Amer Mardini: Suspect in Syrian conflict, Muhammad Ali Durgham Major General: Not an Indonesian name: محمد علي, Jihad Mohamed Sultan Brigadier General: Not an Indonesian name: جهاد محمد سلطان, Mohammed Jabir: Not an Indonesian name: محمد جابر, Mohamed Maaruf Brigadier General: Not an Indonesian name: محمد معروف, Mohamad Fayez Barcha: Not an Indonesian name: محمد فايز برشة, Mohamed Khaddor Major General: Not an Indonesian name: محمد خضور, MuhammadAriLaw: Politician, Muhammad Ari Pratomo, male, born 1982-06-21</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -658,7 +656,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Abdul Aziz: Deceased 1990-06-05, Abdul Aziz: Politician, Abdul Aziz, male, born 1969, Abdul Aziz: Politician, Abdul Aziz, male, born 1972-10-12, Abdul Aziz: Politician, Abdul Aziz, male, born 1970-06-04, in Jakarta for United Development Party, H. ABDUL AZIZ, S.E.: Public figure: Member of Dewan Perwakilan Rakyat (United Development Party Faction), Abdul Azis Suseno: Politician, Abdul Aziz Suseno, male, born 1965-05-10, in Blitar for Prosperous Justice Party, Abdul Azis Halid: Politician, Abdul Azis Halid, male, born 1968-11-25 for Golongan Karya Party, Abdul Azis Khafia: Politician, Abdul Azis Khafia, male, born 1975-11-23, Abdul Azis Hasan: Politician, Abdul Azis Hasan, male, born 1967-06-30, in Ujung Pandang for People's Conscience Party, Sheikh Abdul Aziz: Deceased 2008-08-11, Abdul Aziz Abbasin: Not an Indonesian name: عبد العزيز عباسین, Abdul Aziz Kamis: Politician, Abdul Aziz Kamis, male, born 1961-11-06, Abdul Aziz Junejo: Politician, Abdul Aziz Junejo, male, born 1961-12-07 for Pakistan Peoples Party, Abdul Aziz Mia: Politician, Abdul Aziz Mia, male, born 1955 for Bangladesh Jamaat-e-Islami, Abdul Aziz Khandaker: Deceased 1991, Abdul Aziz Angkat: Deceased 2009-02-03, Aziz Abdullaev: Not an Indonesian name: Азиз Рефатович Абдуллаев, Dawood Ibrahim Kaskar: Foreigner: India</t>
+          <t>Abdul Aziz: Politician, Abdul Aziz, male, born 1969, Abdul Aziz: Deceased 1990-06-05, Abdul Aziz: Politician, Abdul Aziz, male, born 1972-10-12, Abdul Aziz: Politician, Abdul Aziz, male, born 1970-06-04, in Jakarta for United Development Party, H. ABDUL AZIZ, S.E.: Public figure: Member of Dewan Perwakilan Rakyat (United Development Party Faction), Abdul Azis Halid: Politician, Abdul Azis Halid, male, born 1968-11-25 for Golongan Karya Party, Abdul Azis Hasan: Politician, Abdul Azis Hasan, male, born 1967-06-30, in Ujung Pandang for People's Conscience Party, Abdul Azis Khafia: Politician, Abdul Azis Khafia, male, born 1975-11-23, Abdul Azis Suseno: Politician, Abdul Aziz Suseno, male, born 1965-05-10, in Blitar for Prosperous Justice Party, Sheikh Abdul Aziz: Deceased 2008-08-11, Abdul Aziz Abbasin: Not an Indonesian name: عبد العزيز عباسین, Abdul Aziz Angkat: Deceased 2009-02-03, Abdul Aziz Khandaker: Deceased 1991, Abdul Aziz Kamis: Politician, Abdul Aziz Kamis, male, born 1961-11-06, Abdul Aziz Mia: Politician, Abdul Aziz Mia, male, born 1955 for Bangladesh Jamaat-e-Islami, Abdul Aziz Junejo: Politician, Abdul Aziz Junejo, male, born 1961-12-07 for Pakistan Peoples Party, Aziz Abdullaev: Not an Indonesian name: Азиз Рефатович Абдуллаев, Dawood Ibrahim Kaskar: Foreigner: India</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -784,17 +782,15 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Abu Bakar: Deceased 2019-07-13, Abu Bakar Abdi: Politician, Abu Bakar Abdi, male, born 1965-05-05, Wan Abubakar: Politician, Wan Abu Bakar, male, born 1950-08-09, in Selat Panjang for National Mandate Party, Tagore Abubakar: Politician, Tagore Abu Bakar, male, born 1954-04-20, in Takengon for Indonesian Democratic Party – Struggle, Abu Bakar Jamalia: Politician, Abu Bakar Jamalia, male, born 1953-07-21, Wan Abu Bakar: Politician, Wan Abu Bakar, male, born 1950-08-09 for National Mandate Party, Abu Bakar Sidik: Politician, Abu Bakar Sidik, male, born 1962-05-25, Aboe Bakar Al-Habsyi: Politician, Aboe Bakar, Habib Aboe Bakar Alhabsyi, male, born 1964-10-15, in Jakarta for Prosperous Justice Party, Mohammed, Shariff Omar: Foreigner: TANZANIA, UNITED REPUBLIC OF, Abu Bakr Baira: Not an Indonesian name: أبو بكر مصطفى بعيرة</t>
+          <t>Abu Bakar: Deceased 2019-07-13, Wan Abubakar: Politician, Wan Abu Bakar, male, born 1950-08-09, in Selat Panjang for National Mandate Party, Abu Bakar Abdi: Politician, Abu Bakar Abdi, male, born 1965-05-05, Abu Bakar Jamalia: Politician, Abu Bakar Jamalia, male, born 1953-07-21, in Kuala Tungkal, Abu Bakar Sidik: Politician, Abu Bakar Sidik, male, born 1962-05-25, Wan Abu Bakar: Politician, Wan Abu Bakar, male, born 1950-08-09 for National Mandate Party, Tagore Abubakar: Politician, Tagore Abu Bakar, male, born 1954-04-20, in Takengon for Indonesian Democratic Party – Struggle, Aboe Bakar Al-Habsyi: Politician, Aboe Bakar, Habib Aboe Bakar Alhabsyi, male, born 1964-10-15, in Jakarta for Prosperous Justice Party, Mohammed, Shariff Omar: Foreigner: TANZANIA, UNITED REPUBLIC OF, Abu Bakr Baira: Not an Indonesian name: أبو بكر مصطفى بعيرة</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Abu Bakar Ba'asyir: Foreign identifier: QI.B.217.06.
-Sanctions: article 3 paragraphs 1 and 2 (Financial sanctions) and articles 4 and 4a (Travel ban)
+          <t>Abu Bakar Ba'asyir: Foreign identifier: QI.B.217.06.
+Sanctions: Art. 3 Abs. 1 und 2 (Finanzsanktionen) und Art. 4 sowie 4a (Ein- und Durchreiseverbot)
 Other information: Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 Jan 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 Nov 2020. INTERPOL-UN Security Council Special Notice web link available.
-Good quality a.k.a a) Abu Bakar Baasyir, born on 17 Aug 1938 in Jombang, East Java, Indonesia; b) Abu Bakar Bashir born on 17 Aug 1938 in Jombang, East Java, Indonesia, Abu Bakar Ba'asyir: Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020., ABU BAKAR BA'ASYIR: Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals, Abu Bakar Bashir: Abdus Somad, Abu Bakar Baasyir, Abu Bakar Ba’asyir, Abdus Samad, born 1938-08-17, in , Abu Bakar BAASYIR: (UK Sanctions List Ref):AQD0114. (UN Ref):QDi.217. Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/notice/search/un/1428633
-Listed On: 26/04/2006;
-Date Designated: 21/04/2006;, Abu Bakar Bashir: Abdus Somad, Abu Bakar Baasyir, Abu Bakar Ba’asyir, Abdus Samad, male, born 1938-08-17, in </t>
+Good quality a.k.a a) Abu Bakar Baasyir, born on 17 Aug 1938 in Jombang, East Java, Indonesia; b) Abu Bakar Bashir born on 17 Aug 1938 in Jombang, East Java, Indonesia, Abu Bakar Ba'asyir: Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020., ABU BAKAR BA'ASYIR: Formed Jemmah Anshorut Tauhid (JAT) (QDe.133) in 2008. In 2010, arrested for incitement to commit terrorism and fundraising with respect to a training camp in Aceh, Indonesia and sentenced to 15 years in 2011. Ba'asyir was released from prison on 8 January 2021 after serving his sentence in accordance with Indonesian laws and regulations. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2368 (2017) was concluded on 24 November 2020. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals</t>
         </is>
       </c>
     </row>
@@ -840,7 +836,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Mohammad Yahiya Moalla Dr.: Not an Indonesian name: محمد يحيى معلا, Imad Mohammad Deeb Khamis: Not an Indonesian name: عماد محمد ديب خميس, Mohammad Mufleh: Not an Indonesian name: محمد مفلح, Mohammed Bilal Brigadier General: Suspect in Syrian conflict, Mohammad Abdul-Sattar Al Sayed Dr.: Not an Indonesian name: محمد عبد الستار السيد, Ahmad Ballul: Not an Indonesian name: أحمد بالول, Amr Armanazi: Suspect in Syrian conflict, Mohammed Ali Nasr General: Not an Indonesian name: محمد علي نصر, S. Muhammad: Politician, S. Muhammad, male, born 1960-04-25, in Gresik for National Awakening Party, Muhammed Zamrini Brigadier-General: Not an Indonesian name: محمد زمريني, Muhamad: Politician, Muhamad, male, born 1964-04-06, Muhammadong: Politician, Muhammadong, male, born 1969-01-09 for Great Indonesia Movement Party</t>
+          <t>Mohammad Mufleh: Not an Indonesian name: محمد مفلح, Imad Mohammad Deeb Khamis: Not an Indonesian name: عماد محمد ديب خميس, Mohammad Abdul-Sattar Al Sayed Dr.: Not an Indonesian name: محمد عبد الستار السيد, Ahmad Ballul: Not an Indonesian name: أحمد بالول, Mohammed Ali Nasr General: Not an Indonesian name: محمد علي نصر, Mohammad Yahiya Moalla Dr.: Not an Indonesian name: محمد يحيى معلا, Amr Armanazi: Suspect in Syrian conflict, Mohammed Bilal Brigadier General: Suspect in Syrian conflict, S. Muhammad: Politician, S. Muhammad, male, born 1960-04-25, in Gresik for National Awakening Party, Muhammed Zamrini Brigadier-General: Not an Indonesian name: محمد زمريني, Muhamad: Politician, Muhamad, male, born 1964-04-06, Muhammadong: Politician, Muhammadong, male, born 1969-01-09 for Great Indonesia Movement Party</t>
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
@@ -887,7 +883,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Ali Abdullah Ayyub: Not an Indonesian name: علي عبدالله أيوب, Abdullah Khaleel Hussein: Not an Indonesian name: عبدالله خليل حسين, Abdullah Berri: Not an Indonesian name: عبدالله بري, MUSA HILAL ABDALLA ALNSIEM: Foreigner: Sudan, ABDALLAH: Suspect in Syrian conflict, Abdillah: Politician, Abdillah, male, born 1965-05-26, Abdillah: Politician, Abdillah, male, born 1955-05-19, in Medan, Subhi Ahmad Al Abdallah: Not an Indonesian name: صبحي أحمد العبدالله, Suhail Al-Abdullah Brigadier General: Not an Indonesian name: سهيل العبدالله, Khalaf Souleymane Abdallah: Suspect in Syrian conflict, AL-ABDALLAH: Suspect in Syrian conflict</t>
+          <t>Ali Abdullah Ayyub: Not an Indonesian name: علي عبدالله أيوب, Abdullah Khaleel Hussein: Not an Indonesian name: عبدالله خليل حسين, Abdullah Berri: Not an Indonesian name: عبدالله بري, MUSA HILAL ABDALLA ALNSIEM: Foreigner: Sudan, ABDALLAH: Suspect in Syrian conflict, Abdillah: Politician, Abdillah, male, born 1965-05-26, Abdillah: Politician, Abdillah, male, born 1955-05-19, in Medan, Suhail Al-Abdullah Brigadier General: Not an Indonesian name: سهيل العبدالله, Subhi Ahmad Al Abdallah: Not an Indonesian name: صبحي أحمد العبدالله, Khalaf Souleymane Abdallah: Suspect in Syrian conflict, AL-ABDALLAH: Suspect in Syrian conflict</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -938,7 +934,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Suhayl Hassan: Suspect in Syrian conflict, Malik Hasan: Not an Indonesian name: مالك حسن, Hossein Taeb: Not an Indonesian name: حسين طائب, Hasani: Deceased 2018-02-17, M. M. Hassan: Politician, Malik Mohammed Hassan, male, born 1947-05-14, in Thiruvananthapuram for Indian National Congress, Bassam Al Hassan: Not an Indonesian name: بسام الحسن, Ibrahim Al-Hassan Major General: Not an Indonesian name: إبراهيم الحسن, AL-HASAN: Suspect in Syrian conflict, Jamil Hassan: Not an Indonesian name: جميل حسن, Nabil Al-Hasan: Not an Indonesian name: نبيل الحسن, Nabil AL-HASAN: Not an Indonesian name: حسن نبيل, Ahmed Mahmoud Hassan: Not an Indonesian name: šejk Hassan, Hassan Khan: Politician, Haji Ghulam Hassan Khan, male, born 1936-12-11 for Jammu &amp; Kashmir National Conference</t>
+          <t>Suhayl Hassan: Suspect in Syrian conflict, Malik Hasan: Not an Indonesian name: مالك حسن, Hossein Taeb: Not an Indonesian name: حسين طائب, M. M. Hassan: Politician, Malik Mohammed Hassan, male, born 1947-05-14, in Thiruvananthapuram for Indian National Congress, Hasani: Deceased 2018-02-17, Bassam Al Hassan: Not an Indonesian name: بسام الحسن, Ibrahim Al-Hassan Major General: Not an Indonesian name: إبراهيم الحسن, AL-HASAN: Suspect in Syrian conflict, Jamil Hassan: Not an Indonesian name: جميل حسن, Nabil Al-Hasan: Not an Indonesian name: نبيل الحسن, Nabil AL-HASAN: Not an Indonesian name: حسن نبيل, Ahmed Mahmoud Hassan: Not an Indonesian name: šejk Hassan, Hassan Khan: Politician, Haji Ghulam Hassan Khan, male, born 1936-12-11 for Jammu &amp; Kashmir National Conference</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
@@ -985,7 +981,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Ahmed al-Jarroucheh Major General: Not an Indonesian name: أحمد الجاروشة, Ahmed Khalil Khalil: Not an Indonesian name: احمد خليل خليل, Ghassan Ahmed Ghannam: Suspect in Syrian conflict, Ahmed Dibe: Not an Indonesian name: أحمد ديب, Ahmad: Politician, Ahmad, male, born 1966-11-27, Ahmad Tohari: Politician, Ahmad, male, born 1948-06-13, in , Ahmad Sayyed: Not an Indonesian name: أحمد السيد, Riad al-Ahmed Major General: Not an Indonesian name: رياض الأحمد, Jawdat al-Ahmed Brigadier General: Not an Indonesian name: جودت الأحمد, Mohammed al-Ahmed: Not an Indonesian name: محمد الأحمد, Ahmad AL-SAYED: Suspect in Syrian conflict</t>
+          <t>Ahmed Khalil Khalil: Not an Indonesian name: احمد خليل خليل, Ahmed al-Jarroucheh Major General: Not an Indonesian name: أحمد الجاروشة, Ahmed Dibe: Not an Indonesian name: أحمد ديب, Ghassan Ahmed Ghannam: Suspect in Syrian conflict, Ahmad Tohari: Politician, Ahmad, male, born 1948-06-13, in , Ahmad: Politician, Ahmad, male, born 1966-11-27, Jawdat al-Ahmed Brigadier General: Not an Indonesian name: جودت الأحمد, Mohammed al-Ahmed: Not an Indonesian name: محمد الأحمد, Ahmad Sayyed: Not an Indonesian name: أحمد السيد, Riad al-Ahmed Major General: Not an Indonesian name: رياض الأحمد, Ahmad AL-SAYED: Suspect in Syrian conflict</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1044,7 +1040,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Abdul Razak Ahmad: Deceased 2007, أحمد الشيخ عبدالقادر: Not an Indonesian name: أحمد الشيخ عبدالقادر, Ahmad Sheik Abdul-Qader: Not an Indonesian name: أحمد الشيخ عبد القادر, Ahmad al-Sheik Abdulquader: Not an Indonesian name: أحمد الشيخ عبدالقادر, Subhi Ahmad AL ABDALLAH: Not an Indonesian name: صبحي احمد العبدالله, Subhi Ahmad AL ABDALLAH: Not an Indonesian name: صبحي احمد العبدالله, Abdul Ghafoor Ahmed: Deceased 2012-12-26, Ahmad al-Sheik ABDULQADER: Not an Indonesian name: القادر عبد الشيخ أحمد, Imad Abdullah Sara: Not an Indonesian name: عماد عبدالله سارة</t>
+          <t>أحمد الشيخ عبدالقادر: Not an Indonesian name: أحمد الشيخ عبدالقادر, Ahmad al-Sheik ABDULQADER: Not an Indonesian name: القادر عبد الشيخ أحمد, Ahmad al-Sheik Abdulquader: Not an Indonesian name: أحمد الشيخ عبدالقادر, Abdul Razak Ahmad: Deceased 2007, Ahmad Mufti Salim: Politician, Ahmad Mufti Salim, male, born 1975-08-28, Subhi Ahmad AL ABDALLAH: Not an Indonesian name: صبحي احمد العبدالله, Subhi Ahmad Al-Abdullah: Suspect in Syrian conflict, Subhi Ahmad AL ABDALLAH: Not an Indonesian name: صبحي احمد العبدالله</t>
         </is>
       </c>
       <c r="M11" t="inlineStr"/>
@@ -1096,14 +1092,14 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Mubarok: Yassin Syawal, Salim Yasin, Yasin Mahmud Mochtar, Abdul Hadi Yasin, Muhamad Mubarok, Muhammad Syawal, Yassin Sywal, Abu Seta, Mahmud, Abu Muamar, born 1962-09-03, in , Yassin SYAWAL: Associated With: Al Qaeda;
+          <t>Yassin SYAWAL: Associated With: Al Qaeda;
 NZ Designation Date: 1/21/2004;
 Entry Date2: 25/06/2004
 Amended 12/12/2014 SCA/2/14 (25)
 Amended 29/03/2019 SCA/2/19 (07);
 Sanctions List Permanent Reference Number: QDi.123;
 Other2: At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 Feb. 2019.v Review pursuant to Security Council 
-resolution 2610 (2021) was concluded on 8 November 2022. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/notice/search/un/1424789, Yassin Syawal: At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 Feb. 2019. Review pursuant to Security Council resolution 2610 (2021) was concluded on 8 November 2022., MAHMUD: (UK Sanctions List Ref):AQD0335. (UN Ref):QDi.123. At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 Feb. 2019. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/notice/search/un/1424789
+resolution 2610 (2021) was concluded on 8 November 2022. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/notice/search/un/1424789, Mubarok: Yassin Syawal, Salim Yasin, Yasin Mahmud Mochtar, Abdul Hadi Yasin, Muhamad Mubarok, Muhammad Syawal, Yassin Sywal, Abu Seta, Mahmud, Abu Muamar, born 1962-09-03, in , Yassin Syawal: At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 Feb. 2019. Review pursuant to Security Council resolution 2610 (2021) was concluded on 8 November 2022., MAHMUD: (UK Sanctions List Ref):AQD0335. (UN Ref):QDi.123. At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 Feb. 2019. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/notice/search/un/1424789
 Listed On: 05/09/2003;
 Date Designated: 09/09/2003;, Mubarok: Yassin Syawal, Salim Yasin, Yasin Mahmud Mochtar, Abdul Hadi Yasin, Muhamad Mubarok, Muhammad Syawal, Yassin Sywal, Abu Seta, Mahmud, Abu Muamar, male, born 1962-09-03, in , Yassin SYAWAL: ABU MUAMAR, Yasin Mahmud MOCHTAR, Muhamad MUBAROK, Muhammad SYAWAL, Abdul Hadi YASIN, Salim YASIN, ABU SETA, MAHMUD, Syawal YASIN, Laode Agussalim MUBARAK, Ustad Haji Laudi Agus Salim MUHAMMAD, Mohd Shahwal KHAN, Laode IDA, AGUS SALIM, born 03 Sep 1962, in , YASSIN SYAWAL: At large as at Dec. 2003. Review pursuant to Security Council resolution 1822 (2008) was concluded on 25 May 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 21 February 2019. Review pursuant to Security Council resolution 2610 (2021) was concluded on 8 November 2022. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals</t>
         </is>
@@ -1150,7 +1146,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>False positive</t>
+          <t>Needs explanation</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1158,7 +1154,11 @@
           <t>Ahmad Farhan Hamid: Politician, Ahmad Farhan Hamid, male, born 1953-01-21 for National Mandate Party, Hamid Reza EMADI: Public figure: Former Press TV Newsroom Director. Former Press TV Senior Producer., Fathi Ahmad Hammad: Politician, Fathi Ahmad Hammad, male, born 1961, Najm Hamad AL AHMAD: Not an Indonesian name: نجم حمد الأحمد, Najm Hamad Al Ahmad: Suspect in Syrian conflict, Najm Hamad Al Ahmad: Not an Indonesian name: نجم حمد الأحمد, Najm Hamad AL AHMAD: Not an Indonesian name: نجم حمد الأحمد</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fathi Ahmad Mohammad HAMMAD: Fathi Ahmad HAMMAD, Fathy Ahmed HAMAD, Fathi HAMAD, born 1961, in , Fathi Ahmad Mohammad HAMMAD: Fathi Ahmad HAMMAD, Fathy Ahmed HAMAD, Fathi HAMAD, born 1961, in </t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1310,7 +1310,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Rusmin Abdul Gani: Politician, Rusmin Abdul Gani, male, born 1980-12-08, Abdul Ghani Lone: Deceased 2002-05-21, Ruslan Abdul Gani: Politician, Ruslan Abdul Gani, male, born 1958-12-09 for People's Conscience Party, Emad Abdul-Ghani Sabouni: Not an Indonesian name: عماد عبدالغني صابوني, Abdul Ganie Mohamed: Politician, Abdul Ganie Mohamed, male, born 1937-11-04, Abdul Ghani Baradar: Politician, Baradar, Mullah Abdul Ghani Baradar, male, born 1968-09-29, in Weetmak for Taliban, Abdul Ghani Kasuba: Politician, Abdul Ghani Kasuba, male, born 1951-12-21, in Bacan islands for Prosperous Justice Party</t>
+          <t>Ruslan Abdul Gani: Politician, Ruslan Abdul Gani, male, born 1958-12-09 for People's Conscience Party, Abdul Ghani Lone: Deceased 2002-05-21, Rusmin Abdul Gani: Politician, Rusmin Abdul Gani, male, born 1980-12-08, Emad Abdul-Ghani Sabouni: Not an Indonesian name: عماد عبدالغني صابوني, Abdul Ganie Mohamed: Politician, Abdul Ganie Mohamed, male, born 1937-11-04, Abdul Ghani Kasuba: Politician, Abdul Ghani Kasuba, male, born 1951-12-21, in Bacan islands for Prosperous Justice Party, Abdul Ghani Baradar: Politician, Baradar, Mullah Abdul Ghani Baradar, male, born 1968-09-29, in Weetmak for Taliban</t>
         </is>
       </c>
       <c r="M16" t="inlineStr"/>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Abd Allah Mohamed Ragab Abdel Rahman: Foreigner: Egyptian, Karimi Ahmad Hasan: Not an Indonesian name: Карими Ахмад Хасан, Ahmed Salem HASSAN: Suspect in Syrian conflict, Michel KASSOUHA: Not an Indonesian name: ميشال كسوحة, Michel Kassouha: Suspect in Syrian conflict, Ahmed Mahmoud Hassan: Not an Indonesian name: šejk Hassan, Michel KASSOUHA: Not an Indonesian name: ميشال كسوحة</t>
+          <t>Abd Allah Mohamed Ragab Abdel Rahman: Foreigner: Egyptian, Karimi Ahmad Hasan: Not an Indonesian name: Карими Ахмад Хасан, Ahmed Salem HASSAN: Suspect in Syrian conflict, Michel KASSOUHA: Not an Indonesian name: ميشال كسوحة, Michel Kassouha: Suspect in Syrian conflict, Michel KASSOUHA: Not an Indonesian name: ميشال كسوحة, Ahmed Mahmoud Hassan: Not an Indonesian name: šejk Hassan</t>
         </is>
       </c>
       <c r="M17" t="inlineStr"/>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Mulyadi: Politician, Mulyadi, male, born 1970-11-02, in Bogor for Great Indonesia Movement Party, Mulyadi: Politician, Mulyadi, male, born 1970-03-01, Mulyadi: Politician, Mulyadi, male, born 1963-02-13, in Bukittinggi for Democratic Party, Mulyadi: Politician, Mulyadi, male, born 1967-05-14, in Jakarta for United Development Party, Ir. H. MULYADI: Public figure: Member of Dewan Perwakilan Rakyat (Democrat Party Faction), Muliadi: Politician, Muliadi, male, born 1970-07-07</t>
+          <t>Mulyadi: Politician, Mulyadi, male, born 1963-02-13, in Bukittinggi for Democratic Party, Mulyadi: Politician, Mulyadi, male, born 1967-05-14, in Jakarta for United Development Party, Mulyadi: Politician, Mulyadi, male, born 1970-03-01, Mulyadi: Politician, Mulyadi, male, born 1970-11-02, in Bogor for Great Indonesia Movement Party, Ir. H. MULYADI: Public figure: Member of Dewan Perwakilan Rakyat (Democrat Party Faction), Muliadi: Politician, Muliadi, male, born 1970-07-07</t>
         </is>
       </c>
       <c r="M19" t="inlineStr"/>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Amar Ismael: Not an Indonesian name: عمار إسماعيل, Ismael Ismael: Suspect in Syrian conflict, Ezzedine Ismael: Not an Indonesian name: عزالدين إسماعيل, M. M. Ismail: Deceased 2005-01-17, Ismail: Politician, Ismail, male, born 1957-05-19</t>
+          <t>Amar Ismael: Not an Indonesian name: عمار إسماعيل, Ismael Ismael: Suspect in Syrian conflict, Ezzedine Ismael: Not an Indonesian name: عزالدين إسماعيل, Ismail: Politician, Ismail, male, born 1957-05-19, M. M. Ismail: Deceased 2005-01-17</t>
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Nasrullah: Politician, Nasrullah, male, born 1968-11-18, in Pekalongan for National Mandate Party, Mat Solar: Politician, Nasrullah, male, born 1962-12-04, in Jakarta for United Development Party, Nasrul: Politician, Nasrul, male, born 1967-05-14, Nasrullo Sayidov: Politician, Nasrullo Sayyid), male, born 1958-02-20</t>
+          <t>Mat Solar: Politician, Nasrullah, male, born 1962-12-04, in Jakarta for United Development Party, Nasrullah: Politician, Nasrullah, male, born 1968-11-18, in Pekalongan for National Mandate Party, Nasrul: Politician, Nasrul, male, born 1967-05-14, Nasrullo Sayidov: Politician, Nasrullo Sayyid), male, born 1958-02-20</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -1715,7 +1715,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Rahman: Politician, Rahman, male, born 1962-01-30, in Bandung for United Development Party, A. Rahman: Politician, A. Rahman, male, born 1959-02-17 for United Development Party, K. Rahman Khan: Politician, K. Rahman Khan, male, born 1939-04-05, in Mandya for Indian National Congress, B. Raman: Deceased 2013-06-16</t>
+          <t>A. Rahman: Politician, A. Rahman, male, born 1959-02-17 for United Development Party, Rahman: Politician, Rahman, male, born 1962-01-30, in Bandung for United Development Party, K. Rahman Khan: Politician, K. Rahman Khan, male, born 1939-04-05, in Mandya for Indian National Congress, B. Raman: Deceased 2013-06-16</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>M.K. Anwar: Deceased 2017-10-24, Anwar: Politician, Anwar, male, born 1965-08-05, Anwar: Politician, Anwar, male, born 1963-08-06</t>
+          <t>Anwar: Politician, Anwar, male, born 1965-08-05, Anwar: Politician, Anwar, male, born 1963-08-06, M.K. Anwar: Deceased 2017-10-24</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Samsudin S.: Politician, Samsudin S., male, born 1982-02-12, Samsudin: Politician, Samsudin, male, born 1962-12-01, Syamsudin: Politician, Syamsudin, male, born 1954-02-07, Syamsuddin Hb.: Politician, Syamsuddin Hb., male, born 1974-07-07 for Nasdem Party</t>
+          <t>Samsudin: Politician, Samsudin, male, born 1962-12-01, Samsudin S.: Politician, Samsudin S., male, born 1982-02-12, Syamsudin: Politician, Syamsudin, male, born 1954-02-07, Syamsuddin Hb.: Politician, Syamsuddin Hb., male, born 1974-07-07 for Nasdem Party</t>
         </is>
       </c>
       <c r="M27" t="inlineStr"/>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Sukiman: Politician, Sukiman, male, born 1953-08-10, Sukiman: Politician, Sukiman, male, born 1953-08-10, in Madiun, Sukiman: Politician, Sukiman, male, born 1968-07-15, in Nanga Pak for National Mandate Party, H. SUKIMAN, S. Pd., M.M.: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction)</t>
+          <t>Sukiman: Politician, Sukiman, male, born 1953-08-10, Sukiman: Politician, Sukiman, male, born 1968-07-15, in Nanga Pak for National Mandate Party, Sukiman: Politician, Sukiman, male, born 1953-08-10, in Madiun, H. SUKIMAN, S. Pd., M.M.: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction)</t>
         </is>
       </c>
       <c r="M29" t="inlineStr"/>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Syamsudin: Politician, Syamsudin, male, born 1954-02-07, Syamsuddin Hb.: Politician, Syamsuddin Hb., male, born 1974-07-07 for Nasdem Party, Samsudin S.: Politician, Samsudin S., male, born 1982-02-12, Samsudin: Politician, Samsudin, male, born 1962-12-01</t>
+          <t>Syamsudin: Politician, Syamsudin, male, born 1954-02-07, Syamsuddin Hb.: Politician, Syamsuddin Hb., male, born 1974-07-07 for Nasdem Party, Samsudin: Politician, Samsudin, male, born 1962-12-01, Samsudin S.: Politician, Samsudin S., male, born 1982-02-12</t>
         </is>
       </c>
       <c r="M30" t="inlineStr"/>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Abdul Haris: Politician, Abdul Haris, male, born 1968-05-03, Abdul Haris: Politician, Abdul Haris, male, born 1956-07-11, Abdul Haris Makkie: Politician, Abdul Haris Makkie, male, born 1962-05-10</t>
+          <t>Abdul Haris: Politician, Abdul Haris, male, born 1956-07-11, Abdul Haris: Politician, Abdul Haris, male, born 1968-05-03, Abdul Haris Makkie: Politician, Abdul Haris Makkie, male, born 1962-05-10</t>
         </is>
       </c>
       <c r="M31" t="inlineStr"/>
@@ -2116,12 +2116,12 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Sri Oetari Ratna Dewi: Deceased 2003-11-01</t>
+          <t>Sri Oetari Ratna Dewi: Deceased 2003-11-01, Ratna Juwita Sari: Politician, Ratna Juwita Sari, female, born 1984-03-29, in Tuban for National Awakening Party, Dr. Ratna De: Politician, Dr. Ratna De, female, born 1948-09-06, Ratna Sarah Ayu: Politician, Ratna Sarah Ayu, female, born 1974-09-05, in Jakarta for National Mandate Party</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Dewi Sukarno: Naoko Nemoto, Ratna Sari Dewi Sukarno, female, born 1940-02-06, in Tokyo, Kartika Sari Dewi Soekarno: Kartika Sari Dewi Soekarno, female, born 1967-03-11, in Tokyo</t>
+          <t>Dewi Sukarno: Naoko Nemoto, Ratna Sari Dewi Sukarno, female, born 1940-02-06, in Tokyo</t>
         </is>
       </c>
     </row>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Muslim: Politician, Muslim, male, born 1970-08-12, Muslim: Politician, Muslim, male, born 1971-03-01, in  for Democratic Party, MUSLIM, SHI, MM: Public figure: Member of Dewan Perwakilan Rakyat (Democrat Party Faction)</t>
+          <t>Muslim: Politician, Muslim, male, born 1971-03-01, in  for Democratic Party, Muslim: Politician, Muslim, male, born 1970-08-12, MUSLIM, SHI, MM: Public figure: Member of Dewan Perwakilan Rakyat (Democrat Party Faction)</t>
         </is>
       </c>
       <c r="M38" t="inlineStr"/>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Nasrullah: Politician, Nasrullah, male, born 1968-11-18, in Pekalongan for National Mandate Party, Mat Solar: Politician, Nasrullah, male, born 1962-12-04, in Jakarta for United Development Party</t>
+          <t>Mat Solar: Politician, Nasrullah, male, born 1962-12-04, in Jakarta for United Development Party, Nasrullah: Politician, Nasrullah, male, born 1968-11-18, in Pekalongan for National Mandate Party</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -2560,7 +2560,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Nur'aeni: Politician, Nur'aeni, female, born 1974-10-05 for Democratic Party, Nuraini: Politician, Nuraini, female, born 1989-01-13 for National Awakening Party, Nuraini: Politician, Nuraini, female, born 1973-06-10 for Indonesian Democratic Party – Struggle</t>
+          <t>Nur'aeni: Politician, Nur'aeni, female, born 1974-10-05 for Democratic Party, Nuraini: Politician, Nuraini, female, born 1973-06-10 for Indonesian Democratic Party – Struggle, Nuraini: Politician, Nuraini, female, born 1989-01-13 for National Awakening Party</t>
         </is>
       </c>
       <c r="M41" t="inlineStr"/>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Nuraini: Politician, Nuraini, female, born 1989-01-13 for National Awakening Party, Nuraini: Politician, Nuraini, female, born 1973-06-10 for Indonesian Democratic Party – Struggle, Nur'aeni: Politician, Nur'aeni, female, born 1974-10-05 for Democratic Party</t>
+          <t>Nuraini: Politician, Nuraini, female, born 1973-06-10 for Indonesian Democratic Party – Struggle, Nuraini: Politician, Nuraini, female, born 1989-01-13 for National Awakening Party, Nur'aeni: Politician, Nur'aeni, female, born 1974-10-05 for Democratic Party</t>
         </is>
       </c>
       <c r="M42" t="inlineStr"/>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>T. K. Hamza: Politician, T. K. Hamza, male, born 1937-07-14, in Wandoor for Communist Party of India (Marxist), Muhammad Hamza: Deceased 2021-08-29</t>
+          <t>Muhammad Hamza: Deceased 2021-08-29, T. K. Hamza: Politician, T. K. Hamza, male, born 1937-07-14, in Wandoor for Communist Party of India (Marxist)</t>
         </is>
       </c>
       <c r="M48" t="inlineStr"/>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Ilham: Politician, Ilham, male, born 1968-09-08, Ilham: Politician, Ilham, male, born 1975-05-08</t>
+          <t>Ilham: Politician, Ilham, male, born 1975-05-08, Ilham: Politician, Ilham, male, born 1968-09-08</t>
         </is>
       </c>
       <c r="M50" t="inlineStr"/>
@@ -3034,7 +3034,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>A. R. Iwansyah: Politician, A. R. Iwansyah, male, born 1960-08-11, Iwansyah: Politician, Iwansyah, male, born 1959-07-09</t>
+          <t>Iwansyah: Politician, Iwansyah, male, born 1959-07-09, A. R. Iwansyah: Politician, A. R. Iwansyah, male, born 1960-08-11</t>
         </is>
       </c>
       <c r="M51" t="inlineStr"/>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Amin Ak: Politician, Amin, male, born 1965-07-06 for Prosperous Justice Party, M. Amin: Politician, M. Amin, male, born 1965-09-26</t>
+          <t>M. Amin: Politician, M. Amin, male, born 1965-09-26, Amin Ak: Politician, Amin, male, born 1965-07-06 for Prosperous Justice Party</t>
         </is>
       </c>
       <c r="M55" t="inlineStr"/>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Muhammad Syarifuddin: Politician, M. Syarifuddin, male, born 1954-10-17, in Baturaja, Syarifuddin: Politician, Syarifuddin, male, born 1965-10-19</t>
+          <t>Syarifuddin: Politician, Syarifuddin, male, born 1965-10-19, Muhammad Syarifuddin: Politician, M. Syarifuddin, male, born 1954-10-17, in Baturaja</t>
         </is>
       </c>
       <c r="M60" t="inlineStr"/>
@@ -3613,18 +3613,14 @@
         </is>
       </c>
       <c r="J63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
           <t>False positive</t>
         </is>
       </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>Siti Nurbaya Bakar: Politician, Siti Nurbaya, Dr. Ir. Siti Nurbaya Bakar, M.Sc., female, born 1956-08-28, in Jakarta for Nasdem Party, SITI Nurbaya Bakar: Public figure: Min. of Environment &amp; Forestry</t>
-        </is>
-      </c>
+      <c r="L63" t="inlineStr"/>
       <c r="M63" t="inlineStr"/>
     </row>
     <row r="64">
@@ -3998,7 +3994,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Amin Ak: Politician, Amin, male, born 1965-07-06 for Prosperous Justice Party, M. Amin: Politician, M. Amin, male, born 1965-09-26</t>
+          <t>M. Amin: Politician, M. Amin, male, born 1965-09-26, Amin Ak: Politician, Amin, male, born 1965-07-06 for Prosperous Justice Party</t>
         </is>
       </c>
       <c r="M71" t="inlineStr"/>

</xml_diff>